<commit_message>
this added 30th24 report
</commit_message>
<xml_diff>
--- a/Daily_Work/BL Audit Form.xlsx
+++ b/Daily_Work/BL Audit Form.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24332"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{513DDDBC-A336-42D2-BB64-349D621A787B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B69E8280-114E-478B-B0BC-23716ED22617}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -211,10 +211,10 @@
     <t>Mangrove Communacation</t>
   </si>
   <si>
-    <t xml:space="preserve">29.09.2024 payment </t>
-  </si>
-  <si>
-    <t>28.09.2024</t>
+    <t>30.09.2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">01.10.2024 payment </t>
   </si>
 </sst>
 </file>
@@ -372,24 +372,24 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1324,8 +1324,8 @@
   </sheetPr>
   <dimension ref="A1:F47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1339,19 +1339,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="29" t="s">
-        <v>62</v>
-      </c>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
+      <c r="B1" s="24" t="s">
+        <v>61</v>
+      </c>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
     </row>
     <row r="2" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A2" s="28" t="s">
+      <c r="A2" s="23" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="30" t="s">
@@ -1363,7 +1363,7 @@
       <c r="F2" s="2"/>
     </row>
     <row r="3" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A3" s="28" t="s">
+      <c r="A3" s="23" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
@@ -1375,7 +1375,7 @@
       <c r="F3" s="2"/>
     </row>
     <row r="4" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A4" s="28" t="s">
+      <c r="A4" s="23" t="s">
         <v>28</v>
       </c>
       <c r="B4" s="31" t="s">
@@ -1387,7 +1387,7 @@
       <c r="F4" s="2"/>
     </row>
     <row r="5" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A5" s="28" t="s">
+      <c r="A5" s="23" t="s">
         <v>2</v>
       </c>
       <c r="B5" s="2"/>
@@ -1399,12 +1399,12 @@
       <c r="F5" s="31"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="27"/>
-      <c r="B6" s="27"/>
-      <c r="C6" s="27"/>
-      <c r="D6" s="27"/>
-      <c r="E6" s="27"/>
-      <c r="F6" s="27">
+      <c r="A6" s="22"/>
+      <c r="B6" s="22"/>
+      <c r="C6" s="22"/>
+      <c r="D6" s="22"/>
+      <c r="E6" s="22"/>
+      <c r="F6" s="22">
         <v>1964151517</v>
       </c>
     </row>
@@ -1441,14 +1441,14 @@
         <v>46</v>
       </c>
       <c r="C9" s="2">
-        <v>301203</v>
+        <v>477733</v>
       </c>
       <c r="D9" s="2">
         <v>0.96250000000000002</v>
       </c>
       <c r="E9" s="20">
         <f>C9*D9</f>
-        <v>289907.88750000001</v>
+        <v>459818.01250000001</v>
       </c>
       <c r="F9" s="11"/>
     </row>
@@ -1479,14 +1479,14 @@
         <v>48</v>
       </c>
       <c r="C11" s="2">
-        <v>24730</v>
+        <v>22380</v>
       </c>
       <c r="D11" s="2">
         <v>18.309999999999999</v>
       </c>
       <c r="E11" s="20">
         <f t="shared" si="0"/>
-        <v>452806.3</v>
+        <v>409777.8</v>
       </c>
       <c r="F11" s="12"/>
     </row>
@@ -1498,14 +1498,14 @@
         <v>49</v>
       </c>
       <c r="C12" s="2">
-        <v>266</v>
+        <v>162</v>
       </c>
       <c r="D12" s="2">
         <v>241</v>
       </c>
       <c r="E12" s="20">
         <f t="shared" si="0"/>
-        <v>64106</v>
+        <v>39042</v>
       </c>
       <c r="F12" s="12"/>
     </row>
@@ -1644,7 +1644,7 @@
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
       <c r="E20" s="2">
-        <v>183795</v>
+        <v>41440</v>
       </c>
       <c r="F20" s="12"/>
     </row>
@@ -1658,7 +1658,7 @@
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
       <c r="E21" s="2">
-        <v>7611</v>
+        <v>46791</v>
       </c>
       <c r="F21" s="12"/>
     </row>
@@ -1677,15 +1677,15 @@
       <c r="F22" s="11"/>
     </row>
     <row r="23" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="22" t="s">
+      <c r="A23" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="B23" s="22"/>
-      <c r="C23" s="22"/>
-      <c r="D23" s="22"/>
+      <c r="B23" s="27"/>
+      <c r="C23" s="27"/>
+      <c r="D23" s="27"/>
       <c r="E23" s="20">
         <f>SUM(E9:E22)</f>
-        <v>1456419.7375</v>
+        <v>1455062.3625</v>
       </c>
       <c r="F23" s="11"/>
     </row>
@@ -1699,10 +1699,10 @@
       <c r="A25" s="8">
         <v>15</v>
       </c>
-      <c r="B25" s="23" t="s">
+      <c r="B25" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="C25" s="23"/>
+      <c r="C25" s="28"/>
       <c r="D25" s="9" t="s">
         <v>13</v>
       </c>
@@ -1713,8 +1713,8 @@
       <c r="A26" s="8">
         <v>16</v>
       </c>
-      <c r="B26" s="23"/>
-      <c r="C26" s="23"/>
+      <c r="B26" s="28"/>
+      <c r="C26" s="28"/>
       <c r="D26" s="9" t="s">
         <v>14</v>
       </c>
@@ -1725,13 +1725,13 @@
       <c r="A27" s="8">
         <v>17</v>
       </c>
-      <c r="B27" s="23"/>
-      <c r="C27" s="23"/>
+      <c r="B27" s="28"/>
+      <c r="C27" s="28"/>
       <c r="D27" s="17" t="s">
         <v>56</v>
       </c>
       <c r="E27" s="2">
-        <v>21609</v>
+        <v>28299</v>
       </c>
       <c r="F27" s="11"/>
     </row>
@@ -1739,10 +1739,10 @@
       <c r="A28" s="8">
         <v>18</v>
       </c>
-      <c r="B28" s="24" t="s">
+      <c r="B28" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="C28" s="24"/>
+      <c r="C28" s="29"/>
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
       <c r="F28" s="12"/>
@@ -1751,24 +1751,24 @@
       <c r="A29" s="8">
         <v>19</v>
       </c>
-      <c r="B29" s="24" t="s">
+      <c r="B29" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="C29" s="24"/>
+      <c r="C29" s="29"/>
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
       <c r="F29" s="11"/>
     </row>
     <row r="30" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="22" t="s">
+      <c r="A30" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="B30" s="22"/>
-      <c r="C30" s="22"/>
-      <c r="D30" s="22"/>
+      <c r="B30" s="27"/>
+      <c r="C30" s="27"/>
+      <c r="D30" s="27"/>
       <c r="E30" s="20">
         <f>E23+E29+E28+E27+E26+E25</f>
-        <v>1478028.7375</v>
+        <v>1483361.3625</v>
       </c>
       <c r="F30" s="11"/>
     </row>
@@ -1782,10 +1782,10 @@
       <c r="A32" s="8">
         <v>20</v>
       </c>
-      <c r="B32" s="23" t="s">
+      <c r="B32" s="28" t="s">
         <v>23</v>
       </c>
-      <c r="C32" s="23"/>
+      <c r="C32" s="28"/>
       <c r="D32" s="9" t="s">
         <v>24</v>
       </c>
@@ -1793,15 +1793,15 @@
         <v>400000</v>
       </c>
       <c r="F32" s="21" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="8">
         <v>21</v>
       </c>
-      <c r="B33" s="23"/>
-      <c r="C33" s="23"/>
+      <c r="B33" s="28"/>
+      <c r="C33" s="28"/>
       <c r="D33" s="9" t="s">
         <v>25</v>
       </c>
@@ -1812,8 +1812,8 @@
       <c r="A34" s="8">
         <v>22</v>
       </c>
-      <c r="B34" s="23"/>
-      <c r="C34" s="23"/>
+      <c r="B34" s="28"/>
+      <c r="C34" s="28"/>
       <c r="D34" s="9" t="s">
         <v>26</v>
       </c>
@@ -1821,15 +1821,15 @@
       <c r="F34" s="11"/>
     </row>
     <row r="35" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A35" s="22" t="s">
+      <c r="A35" s="27" t="s">
         <v>27</v>
       </c>
-      <c r="B35" s="22"/>
-      <c r="C35" s="22"/>
-      <c r="D35" s="22"/>
+      <c r="B35" s="27"/>
+      <c r="C35" s="27"/>
+      <c r="D35" s="27"/>
       <c r="E35" s="20">
         <f>E30-E32-E33-E34</f>
-        <v>1078028.7375</v>
+        <v>1083361.3625</v>
       </c>
       <c r="F35" s="11"/>
     </row>
@@ -1936,21 +1936,21 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="C5:F5"/>
+    <mergeCell ref="A30:D30"/>
+    <mergeCell ref="B32:C34"/>
+    <mergeCell ref="A35:D35"/>
+    <mergeCell ref="A23:D23"/>
+    <mergeCell ref="B25:C27"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="B29:C29"/>
     <mergeCell ref="E43:F43"/>
     <mergeCell ref="E44:F44"/>
     <mergeCell ref="E45:F45"/>
     <mergeCell ref="E46:F46"/>
     <mergeCell ref="E47:F47"/>
-    <mergeCell ref="A35:D35"/>
-    <mergeCell ref="A23:D23"/>
-    <mergeCell ref="B25:C27"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="C5:F5"/>
-    <mergeCell ref="A30:D30"/>
-    <mergeCell ref="B32:C34"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="82" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
this adde 01st-24 report
</commit_message>
<xml_diff>
--- a/Daily_Work/BL Audit Form.xlsx
+++ b/Daily_Work/BL Audit Form.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24332"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B69E8280-114E-478B-B0BC-23716ED22617}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{490CB242-551B-40AB-AE20-8A36C82FB82F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -211,10 +211,10 @@
     <t>Mangrove Communacation</t>
   </si>
   <si>
-    <t>30.09.2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">01.10.2024 payment </t>
+    <t>01.10.2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">02.10.2024 payment </t>
   </si>
 </sst>
 </file>
@@ -375,26 +375,26 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1324,8 +1324,8 @@
   </sheetPr>
   <dimension ref="A1:F47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="F33" sqref="F33"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="H33" sqref="H33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1354,12 +1354,12 @@
       <c r="A2" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="30" t="s">
+      <c r="B2" s="25" t="s">
         <v>60</v>
       </c>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="30"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
       <c r="F2" s="2"/>
     </row>
     <row r="3" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
@@ -1378,12 +1378,12 @@
       <c r="A4" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="B4" s="31" t="s">
+      <c r="B4" s="26" t="s">
         <v>59</v>
       </c>
-      <c r="C4" s="31"/>
-      <c r="D4" s="31"/>
-      <c r="E4" s="31"/>
+      <c r="C4" s="26"/>
+      <c r="D4" s="26"/>
+      <c r="E4" s="26"/>
       <c r="F4" s="2"/>
     </row>
     <row r="5" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
@@ -1391,12 +1391,12 @@
         <v>2</v>
       </c>
       <c r="B5" s="2"/>
-      <c r="C5" s="31" t="s">
+      <c r="C5" s="26" t="s">
         <v>58</v>
       </c>
-      <c r="D5" s="31"/>
-      <c r="E5" s="31"/>
-      <c r="F5" s="31"/>
+      <c r="D5" s="26"/>
+      <c r="E5" s="26"/>
+      <c r="F5" s="26"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="22"/>
@@ -1441,14 +1441,14 @@
         <v>46</v>
       </c>
       <c r="C9" s="2">
-        <v>477733</v>
+        <v>390362</v>
       </c>
       <c r="D9" s="2">
         <v>0.96250000000000002</v>
       </c>
       <c r="E9" s="20">
         <f>C9*D9</f>
-        <v>459818.01250000001</v>
+        <v>375723.42499999999</v>
       </c>
       <c r="F9" s="11"/>
     </row>
@@ -1479,14 +1479,14 @@
         <v>48</v>
       </c>
       <c r="C11" s="2">
-        <v>22380</v>
+        <v>20730</v>
       </c>
       <c r="D11" s="2">
         <v>18.309999999999999</v>
       </c>
       <c r="E11" s="20">
         <f t="shared" si="0"/>
-        <v>409777.8</v>
+        <v>379566.3</v>
       </c>
       <c r="F11" s="12"/>
     </row>
@@ -1555,14 +1555,14 @@
         <v>52</v>
       </c>
       <c r="C15" s="2">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D15" s="2">
         <v>100</v>
       </c>
       <c r="E15" s="20">
         <f t="shared" si="0"/>
-        <v>8000</v>
+        <v>7900</v>
       </c>
       <c r="F15" s="12"/>
     </row>
@@ -1644,7 +1644,7 @@
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
       <c r="E20" s="2">
-        <v>41440</v>
+        <v>33565</v>
       </c>
       <c r="F20" s="12"/>
     </row>
@@ -1658,7 +1658,7 @@
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
       <c r="E21" s="2">
-        <v>46791</v>
+        <v>12639</v>
       </c>
       <c r="F21" s="12"/>
     </row>
@@ -1685,7 +1685,7 @@
       <c r="D23" s="27"/>
       <c r="E23" s="20">
         <f>SUM(E9:E22)</f>
-        <v>1455062.3625</v>
+        <v>1298629.2749999999</v>
       </c>
       <c r="F23" s="11"/>
     </row>
@@ -1706,7 +1706,9 @@
       <c r="D25" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="E25" s="2"/>
+      <c r="E25" s="2">
+        <v>44150</v>
+      </c>
       <c r="F25" s="12"/>
     </row>
     <row r="26" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -1718,7 +1720,9 @@
       <c r="D26" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="E26" s="2"/>
+      <c r="E26" s="2">
+        <v>4725</v>
+      </c>
       <c r="F26" s="12"/>
     </row>
     <row r="27" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -1768,7 +1772,7 @@
       <c r="D30" s="27"/>
       <c r="E30" s="20">
         <f>E23+E29+E28+E27+E26+E25</f>
-        <v>1483361.3625</v>
+        <v>1375803.2749999999</v>
       </c>
       <c r="F30" s="11"/>
     </row>
@@ -1790,7 +1794,7 @@
         <v>24</v>
       </c>
       <c r="E32" s="2">
-        <v>400000</v>
+        <v>243000</v>
       </c>
       <c r="F32" s="21" t="s">
         <v>62</v>
@@ -1829,7 +1833,7 @@
       <c r="D35" s="27"/>
       <c r="E35" s="20">
         <f>E30-E32-E33-E34</f>
-        <v>1083361.3625</v>
+        <v>1132803.2749999999</v>
       </c>
       <c r="F35" s="11"/>
     </row>
@@ -1867,8 +1871,8 @@
       <c r="D43" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="E43" s="25"/>
-      <c r="F43" s="25"/>
+      <c r="E43" s="30"/>
+      <c r="F43" s="30"/>
     </row>
     <row r="44" spans="1:6" s="16" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A44" s="14" t="s">
@@ -1883,8 +1887,8 @@
       <c r="D44" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="E44" s="26"/>
-      <c r="F44" s="26"/>
+      <c r="E44" s="31"/>
+      <c r="F44" s="31"/>
     </row>
     <row r="45" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A45" s="10" t="s">
@@ -1899,8 +1903,8 @@
       <c r="D45" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="E45" s="25"/>
-      <c r="F45" s="25"/>
+      <c r="E45" s="30"/>
+      <c r="F45" s="30"/>
     </row>
     <row r="46" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A46" s="10" t="s">
@@ -1915,8 +1919,8 @@
       <c r="D46" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="E46" s="25"/>
-      <c r="F46" s="25"/>
+      <c r="E46" s="30"/>
+      <c r="F46" s="30"/>
     </row>
     <row r="47" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A47" s="10" t="s">
@@ -1931,26 +1935,26 @@
       <c r="D47" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="E47" s="25"/>
-      <c r="F47" s="25"/>
+      <c r="E47" s="30"/>
+      <c r="F47" s="30"/>
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="E43:F43"/>
+    <mergeCell ref="E44:F44"/>
+    <mergeCell ref="E45:F45"/>
+    <mergeCell ref="E46:F46"/>
+    <mergeCell ref="E47:F47"/>
+    <mergeCell ref="A35:D35"/>
+    <mergeCell ref="A23:D23"/>
+    <mergeCell ref="B25:C27"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="B29:C29"/>
     <mergeCell ref="B2:E2"/>
     <mergeCell ref="B4:E4"/>
     <mergeCell ref="C5:F5"/>
     <mergeCell ref="A30:D30"/>
     <mergeCell ref="B32:C34"/>
-    <mergeCell ref="A35:D35"/>
-    <mergeCell ref="A23:D23"/>
-    <mergeCell ref="B25:C27"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="E43:F43"/>
-    <mergeCell ref="E44:F44"/>
-    <mergeCell ref="E45:F45"/>
-    <mergeCell ref="E46:F46"/>
-    <mergeCell ref="E47:F47"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="82" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
this added by 17-11-24
</commit_message>
<xml_diff>
--- a/Daily_Work/BL Audit Form.xlsx
+++ b/Daily_Work/BL Audit Form.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24332"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38C18F3A-84AF-4717-A4F3-352C800D9300}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10EDC595-8E33-41FB-A680-57B0EB203097}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -226,7 +226,7 @@
     <t xml:space="preserve">17.11.2024 payment </t>
   </si>
   <si>
-    <t>16.11.2024</t>
+    <t>17.11.2024</t>
   </si>
 </sst>
 </file>
@@ -428,35 +428,35 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1386,8 +1386,8 @@
   </sheetPr>
   <dimension ref="A1:F51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="I37" sqref="I37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1416,12 +1416,12 @@
       <c r="A2" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="29" t="s">
+      <c r="B2" s="37" t="s">
         <v>60</v>
       </c>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29"/>
-      <c r="E2" s="29"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
       <c r="F2" s="2"/>
     </row>
     <row r="3" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
@@ -1440,12 +1440,12 @@
       <c r="A4" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="B4" s="30" t="s">
+      <c r="B4" s="38" t="s">
         <v>59</v>
       </c>
-      <c r="C4" s="30"/>
-      <c r="D4" s="30"/>
-      <c r="E4" s="30"/>
+      <c r="C4" s="38"/>
+      <c r="D4" s="38"/>
+      <c r="E4" s="38"/>
       <c r="F4" s="2"/>
     </row>
     <row r="5" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
@@ -1453,12 +1453,12 @@
         <v>2</v>
       </c>
       <c r="B5" s="2"/>
-      <c r="C5" s="30" t="s">
+      <c r="C5" s="38" t="s">
         <v>58</v>
       </c>
-      <c r="D5" s="30"/>
-      <c r="E5" s="30"/>
-      <c r="F5" s="30"/>
+      <c r="D5" s="38"/>
+      <c r="E5" s="38"/>
+      <c r="F5" s="38"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="22"/>
@@ -1503,14 +1503,14 @@
         <v>46</v>
       </c>
       <c r="C9" s="2">
-        <v>320058</v>
+        <v>308382</v>
       </c>
       <c r="D9" s="2">
         <v>0.96250000000000002</v>
       </c>
       <c r="E9" s="20">
         <f>C9*D9</f>
-        <v>308055.82500000001</v>
+        <v>296817.67499999999</v>
       </c>
       <c r="F9" s="11"/>
     </row>
@@ -1556,14 +1556,14 @@
         <v>48</v>
       </c>
       <c r="C12" s="2">
-        <v>17510</v>
+        <v>12620</v>
       </c>
       <c r="D12" s="2">
         <v>18.309999999999999</v>
       </c>
       <c r="E12" s="20">
         <f t="shared" si="0"/>
-        <v>320608.09999999998</v>
+        <v>231072.19999999998</v>
       </c>
       <c r="F12" s="12"/>
     </row>
@@ -1632,14 +1632,14 @@
         <v>51</v>
       </c>
       <c r="C16" s="2">
-        <v>51</v>
+        <v>18</v>
       </c>
       <c r="D16" s="2">
         <v>323</v>
       </c>
       <c r="E16" s="20">
         <f t="shared" si="0"/>
-        <v>16473</v>
+        <v>5814</v>
       </c>
       <c r="F16" s="12"/>
     </row>
@@ -1651,14 +1651,14 @@
         <v>52</v>
       </c>
       <c r="C17" s="2">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D17" s="2">
         <v>100</v>
       </c>
       <c r="E17" s="20">
         <f t="shared" si="0"/>
-        <v>7000</v>
+        <v>6900</v>
       </c>
       <c r="F17" s="12"/>
     </row>
@@ -1686,15 +1686,13 @@
       <c r="B19" s="19" t="s">
         <v>54</v>
       </c>
-      <c r="C19" s="2">
-        <v>9</v>
-      </c>
+      <c r="C19" s="2"/>
       <c r="D19" s="2">
         <v>66.412499999999994</v>
       </c>
       <c r="E19" s="20">
         <f t="shared" si="0"/>
-        <v>597.71249999999998</v>
+        <v>0</v>
       </c>
       <c r="F19" s="12"/>
     </row>
@@ -1738,7 +1736,7 @@
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
       <c r="E22" s="2">
-        <v>215320</v>
+        <v>14519</v>
       </c>
       <c r="F22" s="12"/>
     </row>
@@ -1752,7 +1750,7 @@
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
       <c r="E23" s="2">
-        <v>9272</v>
+        <v>23022</v>
       </c>
       <c r="F23" s="12"/>
     </row>
@@ -1771,15 +1769,15 @@
       <c r="F24" s="11"/>
     </row>
     <row r="25" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="31" t="s">
+      <c r="A25" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="B25" s="31"/>
-      <c r="C25" s="31"/>
-      <c r="D25" s="31"/>
+      <c r="B25" s="32"/>
+      <c r="C25" s="32"/>
+      <c r="D25" s="32"/>
       <c r="E25" s="20">
         <f>SUM(E9:E24)</f>
-        <v>1300301.6375000002</v>
+        <v>1001119.875</v>
       </c>
       <c r="F25" s="11"/>
     </row>
@@ -1793,10 +1791,10 @@
       <c r="A27" s="8">
         <v>17</v>
       </c>
-      <c r="B27" s="32" t="s">
+      <c r="B27" s="33" t="s">
         <v>12</v>
       </c>
-      <c r="C27" s="32"/>
+      <c r="C27" s="33"/>
       <c r="D27" s="9" t="s">
         <v>13</v>
       </c>
@@ -1809,8 +1807,8 @@
       <c r="A28" s="8">
         <v>18</v>
       </c>
-      <c r="B28" s="32"/>
-      <c r="C28" s="32"/>
+      <c r="B28" s="33"/>
+      <c r="C28" s="33"/>
       <c r="D28" s="9" t="s">
         <v>14</v>
       </c>
@@ -1821,8 +1819,8 @@
       <c r="A29" s="8">
         <v>19</v>
       </c>
-      <c r="B29" s="32"/>
-      <c r="C29" s="32"/>
+      <c r="B29" s="33"/>
+      <c r="C29" s="33"/>
       <c r="D29" s="17" t="s">
         <v>56</v>
       </c>
@@ -1854,15 +1852,15 @@
       <c r="F31" s="11"/>
     </row>
     <row r="32" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="31" t="s">
+      <c r="A32" s="32" t="s">
         <v>19</v>
       </c>
-      <c r="B32" s="31"/>
-      <c r="C32" s="31"/>
-      <c r="D32" s="31"/>
+      <c r="B32" s="32"/>
+      <c r="C32" s="32"/>
+      <c r="D32" s="32"/>
       <c r="E32" s="20">
         <f>E25+E31+E30+E29+E28+E27</f>
-        <v>1311551.6375000002</v>
+        <v>1012369.875</v>
       </c>
       <c r="F32" s="11"/>
     </row>
@@ -1876,15 +1874,15 @@
       <c r="A34" s="8">
         <v>22</v>
       </c>
-      <c r="B34" s="32" t="s">
+      <c r="B34" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="C34" s="32"/>
+      <c r="C34" s="33"/>
       <c r="D34" s="9" t="s">
         <v>24</v>
       </c>
       <c r="E34" s="2">
-        <v>400000</v>
+        <v>100000</v>
       </c>
       <c r="F34" s="21" t="s">
         <v>65</v>
@@ -1894,8 +1892,8 @@
       <c r="A35" s="8">
         <v>23</v>
       </c>
-      <c r="B35" s="32"/>
-      <c r="C35" s="32"/>
+      <c r="B35" s="33"/>
+      <c r="C35" s="33"/>
       <c r="D35" s="9" t="s">
         <v>25</v>
       </c>
@@ -1906,8 +1904,8 @@
       <c r="A36" s="8">
         <v>24</v>
       </c>
-      <c r="B36" s="32"/>
-      <c r="C36" s="32"/>
+      <c r="B36" s="33"/>
+      <c r="C36" s="33"/>
       <c r="D36" s="9" t="s">
         <v>26</v>
       </c>
@@ -1918,8 +1916,8 @@
       <c r="A37" s="8">
         <v>25</v>
       </c>
-      <c r="B37" s="32"/>
-      <c r="C37" s="32"/>
+      <c r="B37" s="33"/>
+      <c r="C37" s="33"/>
       <c r="D37" s="25" t="s">
         <v>62</v>
       </c>
@@ -1935,20 +1933,20 @@
       <c r="D38" s="36"/>
       <c r="E38" s="26">
         <f>SUM(E34:E37)</f>
-        <v>400000</v>
+        <v>100000</v>
       </c>
       <c r="F38" s="11"/>
     </row>
     <row r="39" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A39" s="33" t="s">
+      <c r="A39" s="31" t="s">
         <v>27</v>
       </c>
-      <c r="B39" s="33"/>
-      <c r="C39" s="33"/>
-      <c r="D39" s="33"/>
+      <c r="B39" s="31"/>
+      <c r="C39" s="31"/>
+      <c r="D39" s="31"/>
       <c r="E39" s="27">
         <f>E32-E34-E35-E37</f>
-        <v>911551.63750000019</v>
+        <v>912369.875</v>
       </c>
       <c r="F39" s="11"/>
     </row>
@@ -1986,8 +1984,8 @@
       <c r="D47" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="E47" s="37"/>
-      <c r="F47" s="37"/>
+      <c r="E47" s="29"/>
+      <c r="F47" s="29"/>
     </row>
     <row r="48" spans="1:6" s="16" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A48" s="14" t="s">
@@ -2002,8 +2000,8 @@
       <c r="D48" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="E48" s="38"/>
-      <c r="F48" s="38"/>
+      <c r="E48" s="30"/>
+      <c r="F48" s="30"/>
     </row>
     <row r="49" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A49" s="10" t="s">
@@ -2018,8 +2016,8 @@
       <c r="D49" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="E49" s="37"/>
-      <c r="F49" s="37"/>
+      <c r="E49" s="29"/>
+      <c r="F49" s="29"/>
     </row>
     <row r="50" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A50" s="10" t="s">
@@ -2034,8 +2032,8 @@
       <c r="D50" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="E50" s="37"/>
-      <c r="F50" s="37"/>
+      <c r="E50" s="29"/>
+      <c r="F50" s="29"/>
     </row>
     <row r="51" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A51" s="10" t="s">
@@ -2050,27 +2048,27 @@
       <c r="D51" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="E51" s="37"/>
-      <c r="F51" s="37"/>
+      <c r="E51" s="29"/>
+      <c r="F51" s="29"/>
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="E47:F47"/>
-    <mergeCell ref="E48:F48"/>
-    <mergeCell ref="E49:F49"/>
-    <mergeCell ref="E50:F50"/>
-    <mergeCell ref="E51:F51"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="C5:F5"/>
+    <mergeCell ref="A32:D32"/>
+    <mergeCell ref="B34:C37"/>
     <mergeCell ref="A39:D39"/>
     <mergeCell ref="A25:D25"/>
     <mergeCell ref="B27:C29"/>
     <mergeCell ref="B30:C30"/>
     <mergeCell ref="B31:C31"/>
     <mergeCell ref="B38:D38"/>
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="C5:F5"/>
-    <mergeCell ref="A32:D32"/>
-    <mergeCell ref="B34:C37"/>
+    <mergeCell ref="E47:F47"/>
+    <mergeCell ref="E48:F48"/>
+    <mergeCell ref="E49:F49"/>
+    <mergeCell ref="E50:F50"/>
+    <mergeCell ref="E51:F51"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="79" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
this added last date 21-11-24
</commit_message>
<xml_diff>
--- a/Daily_Work/BL Audit Form.xlsx
+++ b/Daily_Work/BL Audit Form.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24332"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10EDC595-8E33-41FB-A680-57B0EB203097}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BE367C7-5282-4D5F-A02E-8AC06AE0AF83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="68">
   <si>
     <t>cÖwZôv‡bi bvg :</t>
   </si>
@@ -223,10 +223,13 @@
     <t>29 voice</t>
   </si>
   <si>
-    <t xml:space="preserve">17.11.2024 payment </t>
-  </si>
-  <si>
-    <t>17.11.2024</t>
+    <t>21.11.2024</t>
+  </si>
+  <si>
+    <t>E-life Comm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">24.11.2024 payment </t>
   </si>
 </sst>
 </file>
@@ -1386,8 +1389,8 @@
   </sheetPr>
   <dimension ref="A1:F51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="I37" sqref="I37"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="F35" sqref="F35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1405,7 +1408,7 @@
         <v>9</v>
       </c>
       <c r="B1" s="24" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C1" s="24"/>
       <c r="D1" s="24"/>
@@ -1503,14 +1506,14 @@
         <v>46</v>
       </c>
       <c r="C9" s="2">
-        <v>308382</v>
+        <v>393510</v>
       </c>
       <c r="D9" s="2">
         <v>0.96250000000000002</v>
       </c>
       <c r="E9" s="20">
         <f>C9*D9</f>
-        <v>296817.67499999999</v>
+        <v>378753.375</v>
       </c>
       <c r="F9" s="11"/>
     </row>
@@ -1521,13 +1524,15 @@
       <c r="B10" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="C10" s="2"/>
+      <c r="C10" s="2">
+        <v>1000</v>
+      </c>
       <c r="D10" s="2">
         <v>27.912500000000001</v>
       </c>
       <c r="E10" s="20">
         <f t="shared" ref="E10:E21" si="0">C10*D10</f>
-        <v>0</v>
+        <v>27912.5</v>
       </c>
       <c r="F10" s="12"/>
     </row>
@@ -1556,14 +1561,14 @@
         <v>48</v>
       </c>
       <c r="C12" s="2">
-        <v>12620</v>
+        <v>18000</v>
       </c>
       <c r="D12" s="2">
         <v>18.309999999999999</v>
       </c>
       <c r="E12" s="20">
         <f t="shared" si="0"/>
-        <v>231072.19999999998</v>
+        <v>329580</v>
       </c>
       <c r="F12" s="12"/>
     </row>
@@ -1632,14 +1637,14 @@
         <v>51</v>
       </c>
       <c r="C16" s="2">
-        <v>18</v>
+        <v>75</v>
       </c>
       <c r="D16" s="2">
         <v>323</v>
       </c>
       <c r="E16" s="20">
         <f t="shared" si="0"/>
-        <v>5814</v>
+        <v>24225</v>
       </c>
       <c r="F16" s="12"/>
     </row>
@@ -1736,7 +1741,7 @@
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
       <c r="E22" s="2">
-        <v>14519</v>
+        <v>32554</v>
       </c>
       <c r="F22" s="12"/>
     </row>
@@ -1750,7 +1755,7 @@
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
       <c r="E23" s="2">
-        <v>23022</v>
+        <v>12212</v>
       </c>
       <c r="F23" s="12"/>
     </row>
@@ -1777,7 +1782,7 @@
       <c r="D25" s="32"/>
       <c r="E25" s="20">
         <f>SUM(E9:E24)</f>
-        <v>1001119.875</v>
+        <v>1235111.875</v>
       </c>
       <c r="F25" s="11"/>
     </row>
@@ -1847,8 +1852,12 @@
         <v>15</v>
       </c>
       <c r="C31" s="34"/>
-      <c r="D31" s="2"/>
-      <c r="E31" s="2"/>
+      <c r="D31" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="E31" s="2">
+        <v>70000</v>
+      </c>
       <c r="F31" s="11"/>
     </row>
     <row r="32" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -1860,7 +1869,7 @@
       <c r="D32" s="32"/>
       <c r="E32" s="20">
         <f>E25+E31+E30+E29+E28+E27</f>
-        <v>1012369.875</v>
+        <v>1316361.875</v>
       </c>
       <c r="F32" s="11"/>
     </row>
@@ -1882,10 +1891,10 @@
         <v>24</v>
       </c>
       <c r="E34" s="2">
-        <v>100000</v>
+        <v>400000</v>
       </c>
       <c r="F34" s="21" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -1933,7 +1942,7 @@
       <c r="D38" s="36"/>
       <c r="E38" s="26">
         <f>SUM(E34:E37)</f>
-        <v>100000</v>
+        <v>400000</v>
       </c>
       <c r="F38" s="11"/>
     </row>
@@ -1946,7 +1955,7 @@
       <c r="D39" s="31"/>
       <c r="E39" s="27">
         <f>E32-E34-E35-E37</f>
-        <v>912369.875</v>
+        <v>916361.875</v>
       </c>
       <c r="F39" s="11"/>
     </row>

</xml_diff>

<commit_message>
this added last date 28-11-24
</commit_message>
<xml_diff>
--- a/Daily_Work/BL Audit Form.xlsx
+++ b/Daily_Work/BL Audit Form.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24332"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BE367C7-5282-4D5F-A02E-8AC06AE0AF83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{539CF28C-EB0B-4BED-99E3-E7501E345275}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="67">
   <si>
     <t>cÖwZôv‡bi bvg :</t>
   </si>
@@ -223,13 +223,10 @@
     <t>29 voice</t>
   </si>
   <si>
-    <t>21.11.2024</t>
-  </si>
-  <si>
-    <t>E-life Comm</t>
-  </si>
-  <si>
-    <t xml:space="preserve">24.11.2024 payment </t>
+    <t>28.11.2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">01.12.2024 payment </t>
   </si>
 </sst>
 </file>
@@ -1389,7 +1386,7 @@
   </sheetPr>
   <dimension ref="A1:F51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
       <selection activeCell="F35" sqref="F35"/>
     </sheetView>
   </sheetViews>
@@ -1506,14 +1503,14 @@
         <v>46</v>
       </c>
       <c r="C9" s="2">
-        <v>393510</v>
+        <v>629590</v>
       </c>
       <c r="D9" s="2">
         <v>0.96250000000000002</v>
       </c>
       <c r="E9" s="20">
         <f>C9*D9</f>
-        <v>378753.375</v>
+        <v>605980.375</v>
       </c>
       <c r="F9" s="11"/>
     </row>
@@ -1524,15 +1521,13 @@
       <c r="B10" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="C10" s="2">
-        <v>1000</v>
-      </c>
+      <c r="C10" s="2"/>
       <c r="D10" s="2">
         <v>27.912500000000001</v>
       </c>
       <c r="E10" s="20">
         <f t="shared" ref="E10:E21" si="0">C10*D10</f>
-        <v>27912.5</v>
+        <v>0</v>
       </c>
       <c r="F10" s="12"/>
     </row>
@@ -1561,14 +1556,14 @@
         <v>48</v>
       </c>
       <c r="C12" s="2">
-        <v>18000</v>
+        <v>13570</v>
       </c>
       <c r="D12" s="2">
         <v>18.309999999999999</v>
       </c>
       <c r="E12" s="20">
         <f t="shared" si="0"/>
-        <v>329580</v>
+        <v>248466.69999999998</v>
       </c>
       <c r="F12" s="12"/>
     </row>
@@ -1637,14 +1632,14 @@
         <v>51</v>
       </c>
       <c r="C16" s="2">
-        <v>75</v>
+        <v>10</v>
       </c>
       <c r="D16" s="2">
         <v>323</v>
       </c>
       <c r="E16" s="20">
         <f t="shared" si="0"/>
-        <v>24225</v>
+        <v>3230</v>
       </c>
       <c r="F16" s="12"/>
     </row>
@@ -1656,14 +1651,14 @@
         <v>52</v>
       </c>
       <c r="C17" s="2">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D17" s="2">
         <v>100</v>
       </c>
       <c r="E17" s="20">
         <f t="shared" si="0"/>
-        <v>6900</v>
+        <v>6700</v>
       </c>
       <c r="F17" s="12"/>
     </row>
@@ -1741,7 +1736,7 @@
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
       <c r="E22" s="2">
-        <v>32554</v>
+        <v>22337</v>
       </c>
       <c r="F22" s="12"/>
     </row>
@@ -1755,7 +1750,7 @@
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
       <c r="E23" s="2">
-        <v>12212</v>
+        <v>10377</v>
       </c>
       <c r="F23" s="12"/>
     </row>
@@ -1782,7 +1777,7 @@
       <c r="D25" s="32"/>
       <c r="E25" s="20">
         <f>SUM(E9:E24)</f>
-        <v>1235111.875</v>
+        <v>1320066.075</v>
       </c>
       <c r="F25" s="11"/>
     </row>
@@ -1803,9 +1798,7 @@
       <c r="D27" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="E27" s="2">
-        <v>11250</v>
-      </c>
+      <c r="E27" s="2"/>
       <c r="F27" s="12"/>
     </row>
     <row r="28" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -1852,12 +1845,8 @@
         <v>15</v>
       </c>
       <c r="C31" s="34"/>
-      <c r="D31" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="E31" s="2">
-        <v>70000</v>
-      </c>
+      <c r="D31" s="2"/>
+      <c r="E31" s="2"/>
       <c r="F31" s="11"/>
     </row>
     <row r="32" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -1869,7 +1858,7 @@
       <c r="D32" s="32"/>
       <c r="E32" s="20">
         <f>E25+E31+E30+E29+E28+E27</f>
-        <v>1316361.875</v>
+        <v>1320066.075</v>
       </c>
       <c r="F32" s="11"/>
     </row>
@@ -1894,7 +1883,7 @@
         <v>400000</v>
       </c>
       <c r="F34" s="21" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -1955,7 +1944,7 @@
       <c r="D39" s="31"/>
       <c r="E39" s="27">
         <f>E32-E34-E35-E37</f>
-        <v>916361.875</v>
+        <v>920066.07499999995</v>
       </c>
       <c r="F39" s="11"/>
     </row>

</xml_diff>

<commit_message>
this added last report 18-12-24
</commit_message>
<xml_diff>
--- a/Daily_Work/BL Audit Form.xlsx
+++ b/Daily_Work/BL Audit Form.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24332"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{539CF28C-EB0B-4BED-99E3-E7501E345275}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76082B94-4B33-454A-AEA6-7695208E29F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -223,10 +223,10 @@
     <t>29 voice</t>
   </si>
   <si>
-    <t>28.11.2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">01.12.2024 payment </t>
+    <t>18.12.2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">19.12.2024 payment </t>
   </si>
 </sst>
 </file>
@@ -1386,7 +1386,7 @@
   </sheetPr>
   <dimension ref="A1:F51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
       <selection activeCell="F35" sqref="F35"/>
     </sheetView>
   </sheetViews>
@@ -1503,14 +1503,14 @@
         <v>46</v>
       </c>
       <c r="C9" s="2">
-        <v>629590</v>
+        <v>442423</v>
       </c>
       <c r="D9" s="2">
         <v>0.96250000000000002</v>
       </c>
       <c r="E9" s="20">
         <f>C9*D9</f>
-        <v>605980.375</v>
+        <v>425832.13750000001</v>
       </c>
       <c r="F9" s="11"/>
     </row>
@@ -1521,13 +1521,15 @@
       <c r="B10" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="C10" s="2"/>
+      <c r="C10" s="2">
+        <v>1500</v>
+      </c>
       <c r="D10" s="2">
         <v>27.912500000000001</v>
       </c>
       <c r="E10" s="20">
         <f t="shared" ref="E10:E21" si="0">C10*D10</f>
-        <v>0</v>
+        <v>41868.75</v>
       </c>
       <c r="F10" s="12"/>
     </row>
@@ -1556,14 +1558,14 @@
         <v>48</v>
       </c>
       <c r="C12" s="2">
-        <v>13570</v>
+        <v>2000</v>
       </c>
       <c r="D12" s="2">
         <v>18.309999999999999</v>
       </c>
       <c r="E12" s="20">
         <f t="shared" si="0"/>
-        <v>248466.69999999998</v>
+        <v>36620</v>
       </c>
       <c r="F12" s="12"/>
     </row>
@@ -1575,14 +1577,14 @@
         <v>49</v>
       </c>
       <c r="C13" s="2">
-        <v>73</v>
+        <v>42</v>
       </c>
       <c r="D13" s="2">
         <v>241</v>
       </c>
       <c r="E13" s="20">
         <f t="shared" si="0"/>
-        <v>17593</v>
+        <v>10122</v>
       </c>
       <c r="F13" s="12"/>
     </row>
@@ -1632,14 +1634,14 @@
         <v>51</v>
       </c>
       <c r="C16" s="2">
-        <v>10</v>
+        <v>70</v>
       </c>
       <c r="D16" s="2">
         <v>323</v>
       </c>
       <c r="E16" s="20">
         <f t="shared" si="0"/>
-        <v>3230</v>
+        <v>22610</v>
       </c>
       <c r="F16" s="12"/>
     </row>
@@ -1651,14 +1653,14 @@
         <v>52</v>
       </c>
       <c r="C17" s="2">
-        <v>67</v>
+        <v>78</v>
       </c>
       <c r="D17" s="2">
         <v>100</v>
       </c>
       <c r="E17" s="20">
         <f t="shared" si="0"/>
-        <v>6700</v>
+        <v>7800</v>
       </c>
       <c r="F17" s="12"/>
     </row>
@@ -1736,7 +1738,7 @@
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
       <c r="E22" s="2">
-        <v>22337</v>
+        <v>18833</v>
       </c>
       <c r="F22" s="12"/>
     </row>
@@ -1750,7 +1752,7 @@
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
       <c r="E23" s="2">
-        <v>10377</v>
+        <v>11329</v>
       </c>
       <c r="F23" s="12"/>
     </row>
@@ -1777,7 +1779,7 @@
       <c r="D25" s="32"/>
       <c r="E25" s="20">
         <f>SUM(E9:E24)</f>
-        <v>1320066.075</v>
+        <v>980396.88749999995</v>
       </c>
       <c r="F25" s="11"/>
     </row>
@@ -1798,7 +1800,9 @@
       <c r="D27" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="E27" s="2"/>
+      <c r="E27" s="2">
+        <v>22500</v>
+      </c>
       <c r="F27" s="12"/>
     </row>
     <row r="28" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -1858,7 +1862,7 @@
       <c r="D32" s="32"/>
       <c r="E32" s="20">
         <f>E25+E31+E30+E29+E28+E27</f>
-        <v>1320066.075</v>
+        <v>1002896.8875</v>
       </c>
       <c r="F32" s="11"/>
     </row>
@@ -1880,7 +1884,7 @@
         <v>24</v>
       </c>
       <c r="E34" s="2">
-        <v>400000</v>
+        <v>100000</v>
       </c>
       <c r="F34" s="21" t="s">
         <v>66</v>
@@ -1931,7 +1935,7 @@
       <c r="D38" s="36"/>
       <c r="E38" s="26">
         <f>SUM(E34:E37)</f>
-        <v>400000</v>
+        <v>100000</v>
       </c>
       <c r="F38" s="11"/>
     </row>
@@ -1944,7 +1948,7 @@
       <c r="D39" s="31"/>
       <c r="E39" s="27">
         <f>E32-E34-E35-E37</f>
-        <v>920066.07499999995</v>
+        <v>902896.88749999995</v>
       </c>
       <c r="F39" s="11"/>
     </row>

</xml_diff>

<commit_message>
this added the last report 25-12-24
</commit_message>
<xml_diff>
--- a/Daily_Work/BL Audit Form.xlsx
+++ b/Daily_Work/BL Audit Form.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24332"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76082B94-4B33-454A-AEA6-7695208E29F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6955A5B-24F4-4CFA-81A8-6F60E874C6E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -190,9 +190,6 @@
     <t>49 data</t>
   </si>
   <si>
-    <t>69 data</t>
-  </si>
-  <si>
     <t>9 voice</t>
   </si>
   <si>
@@ -223,10 +220,13 @@
     <t>29 voice</t>
   </si>
   <si>
-    <t>18.12.2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">19.12.2024 payment </t>
+    <t>20 TK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">26.12.2024 payment </t>
+  </si>
+  <si>
+    <t>25.12.2024</t>
   </si>
 </sst>
 </file>
@@ -428,35 +428,35 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1386,8 +1386,8 @@
   </sheetPr>
   <dimension ref="A1:F51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="F35" sqref="F35"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1405,7 +1405,7 @@
         <v>9</v>
       </c>
       <c r="B1" s="24" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C1" s="24"/>
       <c r="D1" s="24"/>
@@ -1416,12 +1416,12 @@
       <c r="A2" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="37" t="s">
-        <v>60</v>
-      </c>
-      <c r="C2" s="37"/>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
+      <c r="B2" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
       <c r="F2" s="2"/>
     </row>
     <row r="3" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
@@ -1429,7 +1429,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
@@ -1440,12 +1440,12 @@
       <c r="A4" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="B4" s="38" t="s">
-        <v>59</v>
-      </c>
-      <c r="C4" s="38"/>
-      <c r="D4" s="38"/>
-      <c r="E4" s="38"/>
+      <c r="B4" s="30" t="s">
+        <v>58</v>
+      </c>
+      <c r="C4" s="30"/>
+      <c r="D4" s="30"/>
+      <c r="E4" s="30"/>
       <c r="F4" s="2"/>
     </row>
     <row r="5" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
@@ -1453,12 +1453,12 @@
         <v>2</v>
       </c>
       <c r="B5" s="2"/>
-      <c r="C5" s="38" t="s">
-        <v>58</v>
-      </c>
-      <c r="D5" s="38"/>
-      <c r="E5" s="38"/>
-      <c r="F5" s="38"/>
+      <c r="C5" s="30" t="s">
+        <v>57</v>
+      </c>
+      <c r="D5" s="30"/>
+      <c r="E5" s="30"/>
+      <c r="F5" s="30"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="22"/>
@@ -1503,14 +1503,14 @@
         <v>46</v>
       </c>
       <c r="C9" s="2">
-        <v>442423</v>
+        <v>451122</v>
       </c>
       <c r="D9" s="2">
         <v>0.96250000000000002</v>
       </c>
       <c r="E9" s="20">
         <f>C9*D9</f>
-        <v>425832.13750000001</v>
+        <v>434204.92499999999</v>
       </c>
       <c r="F9" s="11"/>
     </row>
@@ -1521,15 +1521,13 @@
       <c r="B10" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="C10" s="2">
-        <v>1500</v>
-      </c>
+      <c r="C10" s="2"/>
       <c r="D10" s="2">
         <v>27.912500000000001</v>
       </c>
       <c r="E10" s="20">
         <f t="shared" ref="E10:E21" si="0">C10*D10</f>
-        <v>41868.75</v>
+        <v>0</v>
       </c>
       <c r="F10" s="12"/>
     </row>
@@ -1538,7 +1536,7 @@
         <v>3</v>
       </c>
       <c r="B11" s="18" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C11" s="2"/>
       <c r="D11" s="2">
@@ -1593,17 +1591,17 @@
         <v>6</v>
       </c>
       <c r="B14" s="19" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C14" s="2">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="D14" s="2">
         <v>470</v>
       </c>
       <c r="E14" s="20">
         <f t="shared" si="0"/>
-        <v>4700</v>
+        <v>11750</v>
       </c>
       <c r="F14" s="12"/>
     </row>
@@ -1634,14 +1632,14 @@
         <v>51</v>
       </c>
       <c r="C16" s="2">
-        <v>70</v>
+        <v>40</v>
       </c>
       <c r="D16" s="2">
         <v>323</v>
       </c>
       <c r="E16" s="20">
         <f t="shared" si="0"/>
-        <v>22610</v>
+        <v>12920</v>
       </c>
       <c r="F16" s="12"/>
     </row>
@@ -1653,14 +1651,14 @@
         <v>52</v>
       </c>
       <c r="C17" s="2">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D17" s="2">
         <v>100</v>
       </c>
       <c r="E17" s="20">
         <f t="shared" si="0"/>
-        <v>7800</v>
+        <v>7500</v>
       </c>
       <c r="F17" s="12"/>
     </row>
@@ -1686,15 +1684,17 @@
         <v>11</v>
       </c>
       <c r="B19" s="19" t="s">
-        <v>54</v>
-      </c>
-      <c r="C19" s="2"/>
+        <v>64</v>
+      </c>
+      <c r="C19" s="2">
+        <v>500</v>
+      </c>
       <c r="D19" s="2">
-        <v>66.412499999999994</v>
+        <v>19.3</v>
       </c>
       <c r="E19" s="20">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>9650</v>
       </c>
       <c r="F19" s="12"/>
     </row>
@@ -1703,7 +1703,7 @@
         <v>12</v>
       </c>
       <c r="B20" s="19" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C20" s="2"/>
       <c r="D20" s="2">
@@ -1738,7 +1738,7 @@
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
       <c r="E22" s="2">
-        <v>18833</v>
+        <v>166863</v>
       </c>
       <c r="F22" s="12"/>
     </row>
@@ -1752,7 +1752,7 @@
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
       <c r="E23" s="2">
-        <v>11329</v>
+        <v>15869</v>
       </c>
       <c r="F23" s="12"/>
     </row>
@@ -1771,15 +1771,15 @@
       <c r="F24" s="11"/>
     </row>
     <row r="25" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="32" t="s">
+      <c r="A25" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="B25" s="32"/>
-      <c r="C25" s="32"/>
-      <c r="D25" s="32"/>
+      <c r="B25" s="31"/>
+      <c r="C25" s="31"/>
+      <c r="D25" s="31"/>
       <c r="E25" s="20">
         <f>SUM(E9:E24)</f>
-        <v>980396.88749999995</v>
+        <v>1106180.925</v>
       </c>
       <c r="F25" s="11"/>
     </row>
@@ -1793,24 +1793,22 @@
       <c r="A27" s="8">
         <v>17</v>
       </c>
-      <c r="B27" s="33" t="s">
+      <c r="B27" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="C27" s="33"/>
+      <c r="C27" s="32"/>
       <c r="D27" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="E27" s="2">
-        <v>22500</v>
-      </c>
+      <c r="E27" s="2"/>
       <c r="F27" s="12"/>
     </row>
     <row r="28" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="8">
         <v>18</v>
       </c>
-      <c r="B28" s="33"/>
-      <c r="C28" s="33"/>
+      <c r="B28" s="32"/>
+      <c r="C28" s="32"/>
       <c r="D28" s="9" t="s">
         <v>14</v>
       </c>
@@ -1821,10 +1819,10 @@
       <c r="A29" s="8">
         <v>19</v>
       </c>
-      <c r="B29" s="33"/>
-      <c r="C29" s="33"/>
+      <c r="B29" s="32"/>
+      <c r="C29" s="32"/>
       <c r="D29" s="17" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E29" s="2"/>
       <c r="F29" s="11"/>
@@ -1854,15 +1852,15 @@
       <c r="F31" s="11"/>
     </row>
     <row r="32" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="32" t="s">
+      <c r="A32" s="31" t="s">
         <v>19</v>
       </c>
-      <c r="B32" s="32"/>
-      <c r="C32" s="32"/>
-      <c r="D32" s="32"/>
+      <c r="B32" s="31"/>
+      <c r="C32" s="31"/>
+      <c r="D32" s="31"/>
       <c r="E32" s="20">
         <f>E25+E31+E30+E29+E28+E27</f>
-        <v>1002896.8875</v>
+        <v>1106180.925</v>
       </c>
       <c r="F32" s="11"/>
     </row>
@@ -1876,26 +1874,26 @@
       <c r="A34" s="8">
         <v>22</v>
       </c>
-      <c r="B34" s="33" t="s">
+      <c r="B34" s="32" t="s">
         <v>23</v>
       </c>
-      <c r="C34" s="33"/>
+      <c r="C34" s="32"/>
       <c r="D34" s="9" t="s">
         <v>24</v>
       </c>
       <c r="E34" s="2">
-        <v>100000</v>
+        <v>200000</v>
       </c>
       <c r="F34" s="21" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="8">
         <v>23</v>
       </c>
-      <c r="B35" s="33"/>
-      <c r="C35" s="33"/>
+      <c r="B35" s="32"/>
+      <c r="C35" s="32"/>
       <c r="D35" s="9" t="s">
         <v>25</v>
       </c>
@@ -1906,8 +1904,8 @@
       <c r="A36" s="8">
         <v>24</v>
       </c>
-      <c r="B36" s="33"/>
-      <c r="C36" s="33"/>
+      <c r="B36" s="32"/>
+      <c r="C36" s="32"/>
       <c r="D36" s="9" t="s">
         <v>26</v>
       </c>
@@ -1918,10 +1916,10 @@
       <c r="A37" s="8">
         <v>25</v>
       </c>
-      <c r="B37" s="33"/>
-      <c r="C37" s="33"/>
+      <c r="B37" s="32"/>
+      <c r="C37" s="32"/>
       <c r="D37" s="25" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E37" s="2"/>
       <c r="F37" s="11"/>
@@ -1929,26 +1927,26 @@
     <row r="38" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="28"/>
       <c r="B38" s="35" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C38" s="35"/>
       <c r="D38" s="36"/>
       <c r="E38" s="26">
         <f>SUM(E34:E37)</f>
-        <v>100000</v>
+        <v>200000</v>
       </c>
       <c r="F38" s="11"/>
     </row>
     <row r="39" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A39" s="31" t="s">
+      <c r="A39" s="33" t="s">
         <v>27</v>
       </c>
-      <c r="B39" s="31"/>
-      <c r="C39" s="31"/>
-      <c r="D39" s="31"/>
+      <c r="B39" s="33"/>
+      <c r="C39" s="33"/>
+      <c r="D39" s="33"/>
       <c r="E39" s="27">
         <f>E32-E34-E35-E37</f>
-        <v>902896.88749999995</v>
+        <v>906180.92500000005</v>
       </c>
       <c r="F39" s="11"/>
     </row>
@@ -1986,8 +1984,8 @@
       <c r="D47" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="E47" s="29"/>
-      <c r="F47" s="29"/>
+      <c r="E47" s="37"/>
+      <c r="F47" s="37"/>
     </row>
     <row r="48" spans="1:6" s="16" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A48" s="14" t="s">
@@ -2002,8 +2000,8 @@
       <c r="D48" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="E48" s="30"/>
-      <c r="F48" s="30"/>
+      <c r="E48" s="38"/>
+      <c r="F48" s="38"/>
     </row>
     <row r="49" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A49" s="10" t="s">
@@ -2018,8 +2016,8 @@
       <c r="D49" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="E49" s="29"/>
-      <c r="F49" s="29"/>
+      <c r="E49" s="37"/>
+      <c r="F49" s="37"/>
     </row>
     <row r="50" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A50" s="10" t="s">
@@ -2034,8 +2032,8 @@
       <c r="D50" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="E50" s="29"/>
-      <c r="F50" s="29"/>
+      <c r="E50" s="37"/>
+      <c r="F50" s="37"/>
     </row>
     <row r="51" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A51" s="10" t="s">
@@ -2050,27 +2048,27 @@
       <c r="D51" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="E51" s="29"/>
-      <c r="F51" s="29"/>
+      <c r="E51" s="37"/>
+      <c r="F51" s="37"/>
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="C5:F5"/>
-    <mergeCell ref="A32:D32"/>
-    <mergeCell ref="B34:C37"/>
+    <mergeCell ref="E47:F47"/>
+    <mergeCell ref="E48:F48"/>
+    <mergeCell ref="E49:F49"/>
+    <mergeCell ref="E50:F50"/>
+    <mergeCell ref="E51:F51"/>
     <mergeCell ref="A39:D39"/>
     <mergeCell ref="A25:D25"/>
     <mergeCell ref="B27:C29"/>
     <mergeCell ref="B30:C30"/>
     <mergeCell ref="B31:C31"/>
     <mergeCell ref="B38:D38"/>
-    <mergeCell ref="E47:F47"/>
-    <mergeCell ref="E48:F48"/>
-    <mergeCell ref="E49:F49"/>
-    <mergeCell ref="E50:F50"/>
-    <mergeCell ref="E51:F51"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="C5:F5"/>
+    <mergeCell ref="A32:D32"/>
+    <mergeCell ref="B34:C37"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="79" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
this added last report 30-12-24
</commit_message>
<xml_diff>
--- a/Daily_Work/BL Audit Form.xlsx
+++ b/Daily_Work/BL Audit Form.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24332"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6955A5B-24F4-4CFA-81A8-6F60E874C6E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{906DEA0A-405B-4419-82B4-4A6F8EA9AC3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -223,10 +223,10 @@
     <t>20 TK</t>
   </si>
   <si>
-    <t xml:space="preserve">26.12.2024 payment </t>
-  </si>
-  <si>
-    <t>25.12.2024</t>
+    <t>26.12.2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">29.12.2024 payment </t>
   </si>
 </sst>
 </file>
@@ -428,35 +428,35 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1387,7 +1387,7 @@
   <dimension ref="A1:F51"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+      <selection activeCell="F35" sqref="F35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1405,7 +1405,7 @@
         <v>9</v>
       </c>
       <c r="B1" s="24" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C1" s="24"/>
       <c r="D1" s="24"/>
@@ -1416,12 +1416,12 @@
       <c r="A2" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="29" t="s">
+      <c r="B2" s="37" t="s">
         <v>59</v>
       </c>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29"/>
-      <c r="E2" s="29"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
       <c r="F2" s="2"/>
     </row>
     <row r="3" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
@@ -1440,12 +1440,12 @@
       <c r="A4" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="B4" s="30" t="s">
+      <c r="B4" s="38" t="s">
         <v>58</v>
       </c>
-      <c r="C4" s="30"/>
-      <c r="D4" s="30"/>
-      <c r="E4" s="30"/>
+      <c r="C4" s="38"/>
+      <c r="D4" s="38"/>
+      <c r="E4" s="38"/>
       <c r="F4" s="2"/>
     </row>
     <row r="5" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
@@ -1453,12 +1453,12 @@
         <v>2</v>
       </c>
       <c r="B5" s="2"/>
-      <c r="C5" s="30" t="s">
+      <c r="C5" s="38" t="s">
         <v>57</v>
       </c>
-      <c r="D5" s="30"/>
-      <c r="E5" s="30"/>
-      <c r="F5" s="30"/>
+      <c r="D5" s="38"/>
+      <c r="E5" s="38"/>
+      <c r="F5" s="38"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="22"/>
@@ -1503,14 +1503,14 @@
         <v>46</v>
       </c>
       <c r="C9" s="2">
-        <v>451122</v>
+        <v>510795</v>
       </c>
       <c r="D9" s="2">
         <v>0.96250000000000002</v>
       </c>
       <c r="E9" s="20">
         <f>C9*D9</f>
-        <v>434204.92499999999</v>
+        <v>491640.1875</v>
       </c>
       <c r="F9" s="11"/>
     </row>
@@ -1521,13 +1521,15 @@
       <c r="B10" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="C10" s="2"/>
+      <c r="C10" s="2">
+        <v>500</v>
+      </c>
       <c r="D10" s="2">
         <v>27.912500000000001</v>
       </c>
       <c r="E10" s="20">
         <f t="shared" ref="E10:E21" si="0">C10*D10</f>
-        <v>0</v>
+        <v>13956.25</v>
       </c>
       <c r="F10" s="12"/>
     </row>
@@ -1556,14 +1558,14 @@
         <v>48</v>
       </c>
       <c r="C12" s="2">
-        <v>2000</v>
+        <v>7963</v>
       </c>
       <c r="D12" s="2">
         <v>18.309999999999999</v>
       </c>
       <c r="E12" s="20">
         <f t="shared" si="0"/>
-        <v>36620</v>
+        <v>145802.53</v>
       </c>
       <c r="F12" s="12"/>
     </row>
@@ -1594,14 +1596,14 @@
         <v>60</v>
       </c>
       <c r="C14" s="2">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="D14" s="2">
         <v>470</v>
       </c>
       <c r="E14" s="20">
         <f t="shared" si="0"/>
-        <v>11750</v>
+        <v>7050</v>
       </c>
       <c r="F14" s="12"/>
     </row>
@@ -1632,14 +1634,14 @@
         <v>51</v>
       </c>
       <c r="C16" s="2">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="D16" s="2">
         <v>323</v>
       </c>
       <c r="E16" s="20">
         <f t="shared" si="0"/>
-        <v>12920</v>
+        <v>8075</v>
       </c>
       <c r="F16" s="12"/>
     </row>
@@ -1738,7 +1740,7 @@
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
       <c r="E22" s="2">
-        <v>166863</v>
+        <v>33683</v>
       </c>
       <c r="F22" s="12"/>
     </row>
@@ -1752,7 +1754,7 @@
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
       <c r="E23" s="2">
-        <v>15869</v>
+        <v>12989</v>
       </c>
       <c r="F23" s="12"/>
     </row>
@@ -1771,15 +1773,15 @@
       <c r="F24" s="11"/>
     </row>
     <row r="25" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="31" t="s">
+      <c r="A25" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="B25" s="31"/>
-      <c r="C25" s="31"/>
-      <c r="D25" s="31"/>
+      <c r="B25" s="32"/>
+      <c r="C25" s="32"/>
+      <c r="D25" s="32"/>
       <c r="E25" s="20">
         <f>SUM(E9:E24)</f>
-        <v>1106180.925</v>
+        <v>1141149.9675</v>
       </c>
       <c r="F25" s="11"/>
     </row>
@@ -1793,10 +1795,10 @@
       <c r="A27" s="8">
         <v>17</v>
       </c>
-      <c r="B27" s="32" t="s">
+      <c r="B27" s="33" t="s">
         <v>12</v>
       </c>
-      <c r="C27" s="32"/>
+      <c r="C27" s="33"/>
       <c r="D27" s="9" t="s">
         <v>13</v>
       </c>
@@ -1807,8 +1809,8 @@
       <c r="A28" s="8">
         <v>18</v>
       </c>
-      <c r="B28" s="32"/>
-      <c r="C28" s="32"/>
+      <c r="B28" s="33"/>
+      <c r="C28" s="33"/>
       <c r="D28" s="9" t="s">
         <v>14</v>
       </c>
@@ -1819,8 +1821,8 @@
       <c r="A29" s="8">
         <v>19</v>
       </c>
-      <c r="B29" s="32"/>
-      <c r="C29" s="32"/>
+      <c r="B29" s="33"/>
+      <c r="C29" s="33"/>
       <c r="D29" s="17" t="s">
         <v>55</v>
       </c>
@@ -1852,15 +1854,15 @@
       <c r="F31" s="11"/>
     </row>
     <row r="32" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="31" t="s">
+      <c r="A32" s="32" t="s">
         <v>19</v>
       </c>
-      <c r="B32" s="31"/>
-      <c r="C32" s="31"/>
-      <c r="D32" s="31"/>
+      <c r="B32" s="32"/>
+      <c r="C32" s="32"/>
+      <c r="D32" s="32"/>
       <c r="E32" s="20">
         <f>E25+E31+E30+E29+E28+E27</f>
-        <v>1106180.925</v>
+        <v>1141149.9675</v>
       </c>
       <c r="F32" s="11"/>
     </row>
@@ -1874,26 +1876,26 @@
       <c r="A34" s="8">
         <v>22</v>
       </c>
-      <c r="B34" s="32" t="s">
+      <c r="B34" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="C34" s="32"/>
+      <c r="C34" s="33"/>
       <c r="D34" s="9" t="s">
         <v>24</v>
       </c>
       <c r="E34" s="2">
-        <v>200000</v>
+        <v>235000</v>
       </c>
       <c r="F34" s="21" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="8">
         <v>23</v>
       </c>
-      <c r="B35" s="32"/>
-      <c r="C35" s="32"/>
+      <c r="B35" s="33"/>
+      <c r="C35" s="33"/>
       <c r="D35" s="9" t="s">
         <v>25</v>
       </c>
@@ -1904,8 +1906,8 @@
       <c r="A36" s="8">
         <v>24</v>
       </c>
-      <c r="B36" s="32"/>
-      <c r="C36" s="32"/>
+      <c r="B36" s="33"/>
+      <c r="C36" s="33"/>
       <c r="D36" s="9" t="s">
         <v>26</v>
       </c>
@@ -1916,8 +1918,8 @@
       <c r="A37" s="8">
         <v>25</v>
       </c>
-      <c r="B37" s="32"/>
-      <c r="C37" s="32"/>
+      <c r="B37" s="33"/>
+      <c r="C37" s="33"/>
       <c r="D37" s="25" t="s">
         <v>61</v>
       </c>
@@ -1933,20 +1935,20 @@
       <c r="D38" s="36"/>
       <c r="E38" s="26">
         <f>SUM(E34:E37)</f>
-        <v>200000</v>
+        <v>235000</v>
       </c>
       <c r="F38" s="11"/>
     </row>
     <row r="39" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A39" s="33" t="s">
+      <c r="A39" s="31" t="s">
         <v>27</v>
       </c>
-      <c r="B39" s="33"/>
-      <c r="C39" s="33"/>
-      <c r="D39" s="33"/>
+      <c r="B39" s="31"/>
+      <c r="C39" s="31"/>
+      <c r="D39" s="31"/>
       <c r="E39" s="27">
         <f>E32-E34-E35-E37</f>
-        <v>906180.92500000005</v>
+        <v>906149.96750000003</v>
       </c>
       <c r="F39" s="11"/>
     </row>
@@ -1984,8 +1986,8 @@
       <c r="D47" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="E47" s="37"/>
-      <c r="F47" s="37"/>
+      <c r="E47" s="29"/>
+      <c r="F47" s="29"/>
     </row>
     <row r="48" spans="1:6" s="16" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A48" s="14" t="s">
@@ -2000,8 +2002,8 @@
       <c r="D48" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="E48" s="38"/>
-      <c r="F48" s="38"/>
+      <c r="E48" s="30"/>
+      <c r="F48" s="30"/>
     </row>
     <row r="49" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A49" s="10" t="s">
@@ -2016,8 +2018,8 @@
       <c r="D49" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="E49" s="37"/>
-      <c r="F49" s="37"/>
+      <c r="E49" s="29"/>
+      <c r="F49" s="29"/>
     </row>
     <row r="50" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A50" s="10" t="s">
@@ -2032,8 +2034,8 @@
       <c r="D50" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="E50" s="37"/>
-      <c r="F50" s="37"/>
+      <c r="E50" s="29"/>
+      <c r="F50" s="29"/>
     </row>
     <row r="51" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A51" s="10" t="s">
@@ -2048,27 +2050,27 @@
       <c r="D51" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="E51" s="37"/>
-      <c r="F51" s="37"/>
+      <c r="E51" s="29"/>
+      <c r="F51" s="29"/>
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="E47:F47"/>
-    <mergeCell ref="E48:F48"/>
-    <mergeCell ref="E49:F49"/>
-    <mergeCell ref="E50:F50"/>
-    <mergeCell ref="E51:F51"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="C5:F5"/>
+    <mergeCell ref="A32:D32"/>
+    <mergeCell ref="B34:C37"/>
     <mergeCell ref="A39:D39"/>
     <mergeCell ref="A25:D25"/>
     <mergeCell ref="B27:C29"/>
     <mergeCell ref="B30:C30"/>
     <mergeCell ref="B31:C31"/>
     <mergeCell ref="B38:D38"/>
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="C5:F5"/>
-    <mergeCell ref="A32:D32"/>
-    <mergeCell ref="B34:C37"/>
+    <mergeCell ref="E47:F47"/>
+    <mergeCell ref="E48:F48"/>
+    <mergeCell ref="E49:F49"/>
+    <mergeCell ref="E50:F50"/>
+    <mergeCell ref="E51:F51"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="79" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
added this last report 09-01-25
</commit_message>
<xml_diff>
--- a/Daily_Work/BL Audit Form.xlsx
+++ b/Daily_Work/BL Audit Form.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24332"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{906DEA0A-405B-4419-82B4-4A6F8EA9AC3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40103FB9-B838-4C03-BC59-DFD03544EB7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -223,10 +223,10 @@
     <t>20 TK</t>
   </si>
   <si>
-    <t>26.12.2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">29.12.2024 payment </t>
+    <t>09.01.2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12.01.2025 payment </t>
   </si>
 </sst>
 </file>
@@ -1386,8 +1386,8 @@
   </sheetPr>
   <dimension ref="A1:F51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="F35" sqref="F35"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1503,14 +1503,14 @@
         <v>46</v>
       </c>
       <c r="C9" s="2">
-        <v>510795</v>
+        <v>643543</v>
       </c>
       <c r="D9" s="2">
         <v>0.96250000000000002</v>
       </c>
       <c r="E9" s="20">
         <f>C9*D9</f>
-        <v>491640.1875</v>
+        <v>619410.13750000007</v>
       </c>
       <c r="F9" s="11"/>
     </row>
@@ -1522,14 +1522,14 @@
         <v>47</v>
       </c>
       <c r="C10" s="2">
-        <v>500</v>
+        <v>200</v>
       </c>
       <c r="D10" s="2">
-        <v>27.912500000000001</v>
+        <v>27.97</v>
       </c>
       <c r="E10" s="20">
         <f t="shared" ref="E10:E21" si="0">C10*D10</f>
-        <v>13956.25</v>
+        <v>5594</v>
       </c>
       <c r="F10" s="12"/>
     </row>
@@ -1540,13 +1540,15 @@
       <c r="B11" s="18" t="s">
         <v>63</v>
       </c>
-      <c r="C11" s="2"/>
+      <c r="C11" s="2">
+        <v>2000</v>
+      </c>
       <c r="D11" s="2">
         <v>27.936800000000002</v>
       </c>
       <c r="E11" s="20">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>55873.600000000006</v>
       </c>
       <c r="F11" s="12"/>
     </row>
@@ -1558,14 +1560,14 @@
         <v>48</v>
       </c>
       <c r="C12" s="2">
-        <v>7963</v>
+        <v>7050</v>
       </c>
       <c r="D12" s="2">
-        <v>18.309999999999999</v>
+        <v>18.63</v>
       </c>
       <c r="E12" s="20">
         <f t="shared" si="0"/>
-        <v>145802.53</v>
+        <v>131341.5</v>
       </c>
       <c r="F12" s="12"/>
     </row>
@@ -1577,14 +1579,14 @@
         <v>49</v>
       </c>
       <c r="C13" s="2">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D13" s="2">
         <v>241</v>
       </c>
       <c r="E13" s="20">
         <f t="shared" si="0"/>
-        <v>10122</v>
+        <v>9399</v>
       </c>
       <c r="F13" s="12"/>
     </row>
@@ -1596,14 +1598,14 @@
         <v>60</v>
       </c>
       <c r="C14" s="2">
-        <v>15</v>
+        <v>40</v>
       </c>
       <c r="D14" s="2">
         <v>470</v>
       </c>
       <c r="E14" s="20">
         <f t="shared" si="0"/>
-        <v>7050</v>
+        <v>18800</v>
       </c>
       <c r="F14" s="12"/>
     </row>
@@ -1634,14 +1636,14 @@
         <v>51</v>
       </c>
       <c r="C16" s="2">
-        <v>25</v>
+        <v>36</v>
       </c>
       <c r="D16" s="2">
         <v>323</v>
       </c>
       <c r="E16" s="20">
         <f t="shared" si="0"/>
-        <v>8075</v>
+        <v>11628</v>
       </c>
       <c r="F16" s="12"/>
     </row>
@@ -1653,14 +1655,14 @@
         <v>52</v>
       </c>
       <c r="C17" s="2">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="D17" s="2">
         <v>100</v>
       </c>
       <c r="E17" s="20">
         <f t="shared" si="0"/>
-        <v>7500</v>
+        <v>7100</v>
       </c>
       <c r="F17" s="12"/>
     </row>
@@ -1689,14 +1691,14 @@
         <v>64</v>
       </c>
       <c r="C19" s="2">
-        <v>500</v>
+        <v>320</v>
       </c>
       <c r="D19" s="2">
-        <v>19.3</v>
+        <v>19.48</v>
       </c>
       <c r="E19" s="20">
         <f t="shared" si="0"/>
-        <v>9650</v>
+        <v>6233.6</v>
       </c>
       <c r="F19" s="12"/>
     </row>
@@ -1740,7 +1742,7 @@
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
       <c r="E22" s="2">
-        <v>33683</v>
+        <v>27810</v>
       </c>
       <c r="F22" s="12"/>
     </row>
@@ -1754,7 +1756,7 @@
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
       <c r="E23" s="2">
-        <v>12989</v>
+        <v>14144</v>
       </c>
       <c r="F23" s="12"/>
     </row>
@@ -1781,7 +1783,7 @@
       <c r="D25" s="32"/>
       <c r="E25" s="20">
         <f>SUM(E9:E24)</f>
-        <v>1141149.9675</v>
+        <v>1308015.8374999999</v>
       </c>
       <c r="F25" s="11"/>
     </row>
@@ -1862,7 +1864,7 @@
       <c r="D32" s="32"/>
       <c r="E32" s="20">
         <f>E25+E31+E30+E29+E28+E27</f>
-        <v>1141149.9675</v>
+        <v>1308015.8374999999</v>
       </c>
       <c r="F32" s="11"/>
     </row>
@@ -1884,7 +1886,7 @@
         <v>24</v>
       </c>
       <c r="E34" s="2">
-        <v>235000</v>
+        <v>400000</v>
       </c>
       <c r="F34" s="21" t="s">
         <v>66</v>
@@ -1935,7 +1937,7 @@
       <c r="D38" s="36"/>
       <c r="E38" s="26">
         <f>SUM(E34:E37)</f>
-        <v>235000</v>
+        <v>400000</v>
       </c>
       <c r="F38" s="11"/>
     </row>
@@ -1948,7 +1950,7 @@
       <c r="D39" s="31"/>
       <c r="E39" s="27">
         <f>E32-E34-E35-E37</f>
-        <v>906149.96750000003</v>
+        <v>908015.83749999991</v>
       </c>
       <c r="F39" s="11"/>
     </row>

</xml_diff>

<commit_message>
this added by last report 20-01-25
</commit_message>
<xml_diff>
--- a/Daily_Work/BL Audit Form.xlsx
+++ b/Daily_Work/BL Audit Form.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24332"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40103FB9-B838-4C03-BC59-DFD03544EB7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67CC619E-D8BC-49BD-A91F-ECB8A00F3173}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="67">
   <si>
     <t>cÖwZôv‡bi bvg :</t>
   </si>
@@ -223,10 +223,10 @@
     <t>20 TK</t>
   </si>
   <si>
-    <t>09.01.2025</t>
-  </si>
-  <si>
-    <t xml:space="preserve">12.01.2025 payment </t>
+    <t>19.01.2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20.01.2025 payment </t>
   </si>
 </sst>
 </file>
@@ -299,7 +299,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -364,11 +364,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -428,35 +441,42 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -481,13 +501,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>447675</xdr:colOff>
-      <xdr:row>46</xdr:row>
+      <xdr:row>47</xdr:row>
       <xdr:rowOff>66675</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>619125</xdr:colOff>
-      <xdr:row>46</xdr:row>
+      <xdr:row>47</xdr:row>
       <xdr:rowOff>171450</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -539,13 +559,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>447675</xdr:colOff>
-      <xdr:row>47</xdr:row>
+      <xdr:row>48</xdr:row>
       <xdr:rowOff>161925</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>619125</xdr:colOff>
-      <xdr:row>47</xdr:row>
+      <xdr:row>48</xdr:row>
       <xdr:rowOff>266700</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -597,13 +617,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>447675</xdr:colOff>
-      <xdr:row>48</xdr:row>
+      <xdr:row>49</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>619125</xdr:colOff>
-      <xdr:row>48</xdr:row>
+      <xdr:row>49</xdr:row>
       <xdr:rowOff>142875</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -655,13 +675,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>447675</xdr:colOff>
-      <xdr:row>49</xdr:row>
+      <xdr:row>50</xdr:row>
       <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>619125</xdr:colOff>
-      <xdr:row>49</xdr:row>
+      <xdr:row>50</xdr:row>
       <xdr:rowOff>133350</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -713,13 +733,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>504825</xdr:colOff>
-      <xdr:row>46</xdr:row>
+      <xdr:row>47</xdr:row>
       <xdr:rowOff>47625</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>676275</xdr:colOff>
-      <xdr:row>46</xdr:row>
+      <xdr:row>47</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -771,13 +791,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>504825</xdr:colOff>
-      <xdr:row>47</xdr:row>
+      <xdr:row>48</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>676275</xdr:colOff>
-      <xdr:row>47</xdr:row>
+      <xdr:row>48</xdr:row>
       <xdr:rowOff>257175</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -829,13 +849,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>504825</xdr:colOff>
-      <xdr:row>48</xdr:row>
+      <xdr:row>49</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>676275</xdr:colOff>
-      <xdr:row>48</xdr:row>
+      <xdr:row>49</xdr:row>
       <xdr:rowOff>142875</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -887,13 +907,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>504825</xdr:colOff>
-      <xdr:row>49</xdr:row>
+      <xdr:row>50</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>676275</xdr:colOff>
-      <xdr:row>49</xdr:row>
+      <xdr:row>50</xdr:row>
       <xdr:rowOff>142875</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -945,13 +965,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>447675</xdr:colOff>
-      <xdr:row>50</xdr:row>
+      <xdr:row>51</xdr:row>
       <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>619125</xdr:colOff>
-      <xdr:row>50</xdr:row>
+      <xdr:row>51</xdr:row>
       <xdr:rowOff>133350</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1003,13 +1023,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>504825</xdr:colOff>
-      <xdr:row>50</xdr:row>
+      <xdr:row>51</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>676275</xdr:colOff>
-      <xdr:row>50</xdr:row>
+      <xdr:row>51</xdr:row>
       <xdr:rowOff>142875</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1384,10 +1404,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:F51"/>
+  <dimension ref="A1:F52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="F35" sqref="F35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1416,12 +1436,12 @@
       <c r="A2" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="37" t="s">
+      <c r="B2" s="30" t="s">
         <v>59</v>
       </c>
-      <c r="C2" s="37"/>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="30"/>
       <c r="F2" s="2"/>
     </row>
     <row r="3" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
@@ -1440,12 +1460,12 @@
       <c r="A4" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="B4" s="38" t="s">
+      <c r="B4" s="31" t="s">
         <v>58</v>
       </c>
-      <c r="C4" s="38"/>
-      <c r="D4" s="38"/>
-      <c r="E4" s="38"/>
+      <c r="C4" s="31"/>
+      <c r="D4" s="31"/>
+      <c r="E4" s="31"/>
       <c r="F4" s="2"/>
     </row>
     <row r="5" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
@@ -1453,12 +1473,12 @@
         <v>2</v>
       </c>
       <c r="B5" s="2"/>
-      <c r="C5" s="38" t="s">
+      <c r="C5" s="31" t="s">
         <v>57</v>
       </c>
-      <c r="D5" s="38"/>
-      <c r="E5" s="38"/>
-      <c r="F5" s="38"/>
+      <c r="D5" s="31"/>
+      <c r="E5" s="31"/>
+      <c r="F5" s="31"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="22"/>
@@ -1503,14 +1523,14 @@
         <v>46</v>
       </c>
       <c r="C9" s="2">
-        <v>643543</v>
+        <v>349810</v>
       </c>
       <c r="D9" s="2">
         <v>0.96250000000000002</v>
       </c>
       <c r="E9" s="20">
         <f>C9*D9</f>
-        <v>619410.13750000007</v>
+        <v>336692.125</v>
       </c>
       <c r="F9" s="11"/>
     </row>
@@ -1522,14 +1542,14 @@
         <v>47</v>
       </c>
       <c r="C10" s="2">
-        <v>200</v>
+        <v>500</v>
       </c>
       <c r="D10" s="2">
         <v>27.97</v>
       </c>
       <c r="E10" s="20">
         <f t="shared" ref="E10:E21" si="0">C10*D10</f>
-        <v>5594</v>
+        <v>13985</v>
       </c>
       <c r="F10" s="12"/>
     </row>
@@ -1541,14 +1561,14 @@
         <v>63</v>
       </c>
       <c r="C11" s="2">
-        <v>2000</v>
+        <v>2110</v>
       </c>
       <c r="D11" s="2">
         <v>27.936800000000002</v>
       </c>
       <c r="E11" s="20">
         <f t="shared" si="0"/>
-        <v>55873.600000000006</v>
+        <v>58946.648000000001</v>
       </c>
       <c r="F11" s="12"/>
     </row>
@@ -1560,14 +1580,14 @@
         <v>48</v>
       </c>
       <c r="C12" s="2">
-        <v>7050</v>
+        <v>9500</v>
       </c>
       <c r="D12" s="2">
         <v>18.63</v>
       </c>
       <c r="E12" s="20">
         <f t="shared" si="0"/>
-        <v>131341.5</v>
+        <v>176985</v>
       </c>
       <c r="F12" s="12"/>
     </row>
@@ -1579,14 +1599,14 @@
         <v>49</v>
       </c>
       <c r="C13" s="2">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="D13" s="2">
         <v>241</v>
       </c>
       <c r="E13" s="20">
         <f t="shared" si="0"/>
-        <v>9399</v>
+        <v>7471</v>
       </c>
       <c r="F13" s="12"/>
     </row>
@@ -1616,15 +1636,13 @@
       <c r="B15" s="19" t="s">
         <v>50</v>
       </c>
-      <c r="C15" s="2">
-        <v>2</v>
-      </c>
+      <c r="C15" s="2"/>
       <c r="D15" s="2">
         <v>341</v>
       </c>
       <c r="E15" s="20">
         <f t="shared" si="0"/>
-        <v>682</v>
+        <v>0</v>
       </c>
       <c r="F15" s="12"/>
     </row>
@@ -1636,14 +1654,14 @@
         <v>51</v>
       </c>
       <c r="C16" s="2">
-        <v>36</v>
+        <v>55</v>
       </c>
       <c r="D16" s="2">
         <v>323</v>
       </c>
       <c r="E16" s="20">
         <f t="shared" si="0"/>
-        <v>11628</v>
+        <v>17765</v>
       </c>
       <c r="F16" s="12"/>
     </row>
@@ -1655,14 +1673,14 @@
         <v>52</v>
       </c>
       <c r="C17" s="2">
-        <v>71</v>
+        <v>92</v>
       </c>
       <c r="D17" s="2">
         <v>100</v>
       </c>
       <c r="E17" s="20">
         <f t="shared" si="0"/>
-        <v>7100</v>
+        <v>9200</v>
       </c>
       <c r="F17" s="12"/>
     </row>
@@ -1690,15 +1708,13 @@
       <c r="B19" s="19" t="s">
         <v>64</v>
       </c>
-      <c r="C19" s="2">
-        <v>320</v>
-      </c>
+      <c r="C19" s="2"/>
       <c r="D19" s="2">
         <v>19.48</v>
       </c>
       <c r="E19" s="20">
         <f t="shared" si="0"/>
-        <v>6233.6</v>
+        <v>0</v>
       </c>
       <c r="F19" s="12"/>
     </row>
@@ -1742,7 +1758,7 @@
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
       <c r="E22" s="2">
-        <v>27810</v>
+        <v>14255</v>
       </c>
       <c r="F22" s="12"/>
     </row>
@@ -1756,7 +1772,7 @@
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
       <c r="E23" s="2">
-        <v>14144</v>
+        <v>14834</v>
       </c>
       <c r="F23" s="12"/>
     </row>
@@ -1783,7 +1799,7 @@
       <c r="D25" s="32"/>
       <c r="E25" s="20">
         <f>SUM(E9:E24)</f>
-        <v>1308015.8374999999</v>
+        <v>1068933.773</v>
       </c>
       <c r="F25" s="11"/>
     </row>
@@ -1835,10 +1851,10 @@
       <c r="A30" s="8">
         <v>20</v>
       </c>
-      <c r="B30" s="34" t="s">
+      <c r="B30" s="35" t="s">
         <v>16</v>
       </c>
-      <c r="C30" s="34"/>
+      <c r="C30" s="35"/>
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
       <c r="F30" s="12"/>
@@ -1847,10 +1863,10 @@
       <c r="A31" s="8">
         <v>21</v>
       </c>
-      <c r="B31" s="34" t="s">
+      <c r="B31" s="35" t="s">
         <v>15</v>
       </c>
-      <c r="C31" s="34"/>
+      <c r="C31" s="35"/>
       <c r="D31" s="2"/>
       <c r="E31" s="2"/>
       <c r="F31" s="11"/>
@@ -1864,7 +1880,7 @@
       <c r="D32" s="32"/>
       <c r="E32" s="20">
         <f>E25+E31+E30+E29+E28+E27</f>
-        <v>1308015.8374999999</v>
+        <v>1068933.773</v>
       </c>
       <c r="F32" s="11"/>
     </row>
@@ -1886,7 +1902,7 @@
         <v>24</v>
       </c>
       <c r="E34" s="2">
-        <v>400000</v>
+        <v>176000</v>
       </c>
       <c r="F34" s="21" t="s">
         <v>66</v>
@@ -1929,106 +1945,102 @@
       <c r="F37" s="11"/>
     </row>
     <row r="38" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="28"/>
-      <c r="B38" s="35" t="s">
+      <c r="A38" s="8">
+        <v>26</v>
+      </c>
+      <c r="B38" s="38" t="s">
+        <v>15</v>
+      </c>
+      <c r="C38" s="39"/>
+      <c r="D38" s="29"/>
+      <c r="E38" s="2"/>
+      <c r="F38" s="11"/>
+    </row>
+    <row r="39" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="28"/>
+      <c r="B39" s="36" t="s">
         <v>62</v>
       </c>
-      <c r="C38" s="35"/>
-      <c r="D38" s="36"/>
-      <c r="E38" s="26">
-        <f>SUM(E34:E37)</f>
-        <v>400000</v>
-      </c>
-      <c r="F38" s="11"/>
-    </row>
-    <row r="39" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A39" s="31" t="s">
+      <c r="C39" s="36"/>
+      <c r="D39" s="37"/>
+      <c r="E39" s="26">
+        <f>SUM(E34:E38)</f>
+        <v>176000</v>
+      </c>
+      <c r="F39" s="11"/>
+    </row>
+    <row r="40" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A40" s="34" t="s">
         <v>27</v>
       </c>
-      <c r="B39" s="31"/>
-      <c r="C39" s="31"/>
-      <c r="D39" s="31"/>
-      <c r="E39" s="27">
-        <f>E32-E34-E35-E37</f>
-        <v>908015.83749999991</v>
-      </c>
-      <c r="F39" s="11"/>
-    </row>
-    <row r="43" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="B43" s="4" t="s">
+      <c r="B40" s="34"/>
+      <c r="C40" s="34"/>
+      <c r="D40" s="34"/>
+      <c r="E40" s="27">
+        <f>E32-E34-E35-E36-E37-E38</f>
+        <v>892933.77300000004</v>
+      </c>
+      <c r="F40" s="11"/>
+    </row>
+    <row r="44" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="B44" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="D43" s="4" t="s">
+      <c r="D44" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="F43" s="4" t="s">
+      <c r="F44" s="4" t="s">
         <v>31</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A45" s="10" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="46" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A46" s="10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="47" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A47" s="10" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A48" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="B47" s="10" t="s">
+      <c r="B48" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="C47" s="10" t="s">
+      <c r="C48" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="D47" s="10" t="s">
+      <c r="D48" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="E47" s="29"/>
-      <c r="F47" s="29"/>
-    </row>
-    <row r="48" spans="1:6" s="16" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A48" s="14" t="s">
+      <c r="E48" s="40"/>
+      <c r="F48" s="40"/>
+    </row>
+    <row r="49" spans="1:6" s="16" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A49" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="B48" s="15" t="s">
+      <c r="B49" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="C48" s="14" t="s">
+      <c r="C49" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="D48" s="14" t="s">
+      <c r="D49" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="E48" s="30"/>
-      <c r="F48" s="30"/>
-    </row>
-    <row r="49" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A49" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="B49" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="C49" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="D49" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="E49" s="29"/>
-      <c r="F49" s="29"/>
+      <c r="E49" s="41"/>
+      <c r="F49" s="41"/>
     </row>
     <row r="50" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A50" s="10" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B50" s="10" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C50" s="10" t="s">
         <v>35</v>
@@ -2036,15 +2048,15 @@
       <c r="D50" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="E50" s="29"/>
-      <c r="F50" s="29"/>
+      <c r="E50" s="40"/>
+      <c r="F50" s="40"/>
     </row>
     <row r="51" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A51" s="10" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B51" s="10" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C51" s="10" t="s">
         <v>35</v>
@@ -2052,30 +2064,47 @@
       <c r="D51" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="E51" s="29"/>
-      <c r="F51" s="29"/>
+      <c r="E51" s="40"/>
+      <c r="F51" s="40"/>
+    </row>
+    <row r="52" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A52" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="B52" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="C52" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="D52" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="E52" s="40"/>
+      <c r="F52" s="40"/>
     </row>
   </sheetData>
-  <mergeCells count="16">
+  <mergeCells count="17">
+    <mergeCell ref="E48:F48"/>
+    <mergeCell ref="E49:F49"/>
+    <mergeCell ref="E50:F50"/>
+    <mergeCell ref="E51:F51"/>
+    <mergeCell ref="E52:F52"/>
+    <mergeCell ref="A40:D40"/>
+    <mergeCell ref="A25:D25"/>
+    <mergeCell ref="B27:C29"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="B39:D39"/>
+    <mergeCell ref="B38:C38"/>
     <mergeCell ref="B2:E2"/>
     <mergeCell ref="B4:E4"/>
     <mergeCell ref="C5:F5"/>
     <mergeCell ref="A32:D32"/>
     <mergeCell ref="B34:C37"/>
-    <mergeCell ref="A39:D39"/>
-    <mergeCell ref="A25:D25"/>
-    <mergeCell ref="B27:C29"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="B38:D38"/>
-    <mergeCell ref="E47:F47"/>
-    <mergeCell ref="E48:F48"/>
-    <mergeCell ref="E49:F49"/>
-    <mergeCell ref="E50:F50"/>
-    <mergeCell ref="E51:F51"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="79" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="77" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
this added by last report 02-02-25
</commit_message>
<xml_diff>
--- a/Daily_Work/BL Audit Form.xlsx
+++ b/Daily_Work/BL Audit Form.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24332"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5D8327E-4DE1-4F72-98F5-1EC2DF1E09A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D9DA9C2-53BB-4E27-958E-8520F212C7FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -226,10 +226,10 @@
     <t xml:space="preserve"> </t>
   </si>
   <si>
-    <t>29.01.2025</t>
-  </si>
-  <si>
-    <t xml:space="preserve">30.01.2025 payment </t>
+    <t>02.02.2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">03.02.2025 payment </t>
   </si>
 </sst>
 </file>
@@ -445,41 +445,41 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1409,8 +1409,8 @@
   </sheetPr>
   <dimension ref="A1:I52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="F35" sqref="F35"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1439,12 +1439,12 @@
       <c r="A2" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="40" t="s">
+      <c r="B2" s="30" t="s">
         <v>59</v>
       </c>
-      <c r="C2" s="40"/>
-      <c r="D2" s="40"/>
-      <c r="E2" s="40"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="30"/>
       <c r="F2" s="2"/>
     </row>
     <row r="3" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
@@ -1463,12 +1463,12 @@
       <c r="A4" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="B4" s="41" t="s">
+      <c r="B4" s="31" t="s">
         <v>58</v>
       </c>
-      <c r="C4" s="41"/>
-      <c r="D4" s="41"/>
-      <c r="E4" s="41"/>
+      <c r="C4" s="31"/>
+      <c r="D4" s="31"/>
+      <c r="E4" s="31"/>
       <c r="F4" s="2"/>
     </row>
     <row r="5" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
@@ -1476,12 +1476,12 @@
         <v>2</v>
       </c>
       <c r="B5" s="2"/>
-      <c r="C5" s="41" t="s">
+      <c r="C5" s="31" t="s">
         <v>57</v>
       </c>
-      <c r="D5" s="41"/>
-      <c r="E5" s="41"/>
-      <c r="F5" s="41"/>
+      <c r="D5" s="31"/>
+      <c r="E5" s="31"/>
+      <c r="F5" s="31"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="22"/>
@@ -1526,14 +1526,14 @@
         <v>46</v>
       </c>
       <c r="C9" s="2">
-        <v>342876</v>
+        <v>352677</v>
       </c>
       <c r="D9" s="2">
         <v>0.96250000000000002</v>
       </c>
       <c r="E9" s="20">
         <f>C9*D9</f>
-        <v>330018.15000000002</v>
+        <v>339451.61249999999</v>
       </c>
       <c r="F9" s="11"/>
     </row>
@@ -1544,15 +1544,13 @@
       <c r="B10" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="C10" s="2">
-        <v>190</v>
-      </c>
+      <c r="C10" s="2"/>
       <c r="D10" s="2">
         <v>27.97</v>
       </c>
       <c r="E10" s="20">
         <f t="shared" ref="E10:E21" si="0">C10*D10</f>
-        <v>5314.3</v>
+        <v>0</v>
       </c>
       <c r="F10" s="12"/>
     </row>
@@ -1564,14 +1562,14 @@
         <v>63</v>
       </c>
       <c r="C11" s="2">
-        <v>590</v>
+        <v>450</v>
       </c>
       <c r="D11" s="2">
         <v>27.936800000000002</v>
       </c>
       <c r="E11" s="20">
         <f t="shared" si="0"/>
-        <v>16482.712</v>
+        <v>12571.560000000001</v>
       </c>
       <c r="F11" s="12"/>
     </row>
@@ -1583,14 +1581,14 @@
         <v>48</v>
       </c>
       <c r="C12" s="2">
-        <v>3790</v>
+        <v>1970</v>
       </c>
       <c r="D12" s="2">
         <v>18.63</v>
       </c>
       <c r="E12" s="20">
         <f t="shared" si="0"/>
-        <v>70607.7</v>
+        <v>36701.1</v>
       </c>
       <c r="F12" s="12"/>
     </row>
@@ -1621,14 +1619,14 @@
         <v>60</v>
       </c>
       <c r="C14" s="2">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="D14" s="2">
         <v>470</v>
       </c>
       <c r="E14" s="20">
         <f t="shared" si="0"/>
-        <v>10810</v>
+        <v>5640</v>
       </c>
       <c r="F14" s="12"/>
     </row>
@@ -1657,14 +1655,14 @@
         <v>51</v>
       </c>
       <c r="C16" s="2">
-        <v>44</v>
+        <v>18</v>
       </c>
       <c r="D16" s="2">
         <v>323</v>
       </c>
       <c r="E16" s="20">
         <f t="shared" si="0"/>
-        <v>14212</v>
+        <v>5814</v>
       </c>
       <c r="F16" s="12"/>
     </row>
@@ -1761,7 +1759,7 @@
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
       <c r="E22" s="2">
-        <v>142494</v>
+        <v>142703</v>
       </c>
       <c r="F22" s="12"/>
     </row>
@@ -1775,7 +1773,7 @@
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
       <c r="E23" s="2">
-        <v>13694</v>
+        <v>12074</v>
       </c>
       <c r="F23" s="12"/>
     </row>
@@ -1794,15 +1792,15 @@
       <c r="F24" s="11"/>
     </row>
     <row r="25" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="33" t="s">
+      <c r="A25" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="B25" s="33"/>
-      <c r="C25" s="33"/>
-      <c r="D25" s="33"/>
+      <c r="B25" s="32"/>
+      <c r="C25" s="32"/>
+      <c r="D25" s="32"/>
       <c r="E25" s="20">
         <f>SUM(E9:E24)</f>
-        <v>1019403.862</v>
+        <v>970726.27249999996</v>
       </c>
       <c r="F25" s="11"/>
     </row>
@@ -1816,10 +1814,10 @@
       <c r="A27" s="8">
         <v>17</v>
       </c>
-      <c r="B27" s="34" t="s">
+      <c r="B27" s="33" t="s">
         <v>12</v>
       </c>
-      <c r="C27" s="34"/>
+      <c r="C27" s="33"/>
       <c r="D27" s="9" t="s">
         <v>13</v>
       </c>
@@ -1830,8 +1828,8 @@
       <c r="A28" s="8">
         <v>18</v>
       </c>
-      <c r="B28" s="34"/>
-      <c r="C28" s="34"/>
+      <c r="B28" s="33"/>
+      <c r="C28" s="33"/>
       <c r="D28" s="9" t="s">
         <v>14</v>
       </c>
@@ -1842,8 +1840,8 @@
       <c r="A29" s="8">
         <v>19</v>
       </c>
-      <c r="B29" s="34"/>
-      <c r="C29" s="34"/>
+      <c r="B29" s="33"/>
+      <c r="C29" s="33"/>
       <c r="D29" s="17" t="s">
         <v>55</v>
       </c>
@@ -1871,19 +1869,21 @@
       </c>
       <c r="C31" s="35"/>
       <c r="D31" s="2"/>
-      <c r="E31" s="2"/>
+      <c r="E31" s="2">
+        <v>53000</v>
+      </c>
       <c r="F31" s="11"/>
     </row>
     <row r="32" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="33" t="s">
+      <c r="A32" s="32" t="s">
         <v>19</v>
       </c>
-      <c r="B32" s="33"/>
-      <c r="C32" s="33"/>
-      <c r="D32" s="33"/>
+      <c r="B32" s="32"/>
+      <c r="C32" s="32"/>
+      <c r="D32" s="32"/>
       <c r="E32" s="20">
         <f>E25+E31+E30+E29+E28+E27</f>
-        <v>1019403.862</v>
+        <v>1023726.2725</v>
       </c>
       <c r="F32" s="11"/>
       <c r="I32" t="s">
@@ -1900,15 +1900,15 @@
       <c r="A34" s="8">
         <v>22</v>
       </c>
-      <c r="B34" s="34" t="s">
+      <c r="B34" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="C34" s="34"/>
+      <c r="C34" s="33"/>
       <c r="D34" s="9" t="s">
         <v>24</v>
       </c>
       <c r="E34" s="2">
-        <v>110000</v>
+        <v>112000</v>
       </c>
       <c r="F34" s="21" t="s">
         <v>67</v>
@@ -1918,8 +1918,8 @@
       <c r="A35" s="8">
         <v>23</v>
       </c>
-      <c r="B35" s="34"/>
-      <c r="C35" s="34"/>
+      <c r="B35" s="33"/>
+      <c r="C35" s="33"/>
       <c r="D35" s="9" t="s">
         <v>25</v>
       </c>
@@ -1930,8 +1930,8 @@
       <c r="A36" s="8">
         <v>24</v>
       </c>
-      <c r="B36" s="34"/>
-      <c r="C36" s="34"/>
+      <c r="B36" s="33"/>
+      <c r="C36" s="33"/>
       <c r="D36" s="9" t="s">
         <v>26</v>
       </c>
@@ -1942,8 +1942,8 @@
       <c r="A37" s="8">
         <v>25</v>
       </c>
-      <c r="B37" s="34"/>
-      <c r="C37" s="34"/>
+      <c r="B37" s="33"/>
+      <c r="C37" s="33"/>
       <c r="D37" s="25" t="s">
         <v>61</v>
       </c>
@@ -1971,20 +1971,20 @@
       <c r="D39" s="37"/>
       <c r="E39" s="26">
         <f>SUM(E34:E38)</f>
-        <v>110000</v>
+        <v>112000</v>
       </c>
       <c r="F39" s="11"/>
     </row>
     <row r="40" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A40" s="32" t="s">
+      <c r="A40" s="34" t="s">
         <v>27</v>
       </c>
-      <c r="B40" s="32"/>
-      <c r="C40" s="32"/>
-      <c r="D40" s="32"/>
+      <c r="B40" s="34"/>
+      <c r="C40" s="34"/>
+      <c r="D40" s="34"/>
       <c r="E40" s="27">
         <f>E32-E34-E35-E36-E37-E38</f>
-        <v>909403.86199999996</v>
+        <v>911726.27249999996</v>
       </c>
       <c r="F40" s="11"/>
     </row>
@@ -2022,8 +2022,8 @@
       <c r="D48" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="E48" s="30"/>
-      <c r="F48" s="30"/>
+      <c r="E48" s="40"/>
+      <c r="F48" s="40"/>
     </row>
     <row r="49" spans="1:6" s="16" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A49" s="14" t="s">
@@ -2038,8 +2038,8 @@
       <c r="D49" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="E49" s="31"/>
-      <c r="F49" s="31"/>
+      <c r="E49" s="41"/>
+      <c r="F49" s="41"/>
     </row>
     <row r="50" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A50" s="10" t="s">
@@ -2054,8 +2054,8 @@
       <c r="D50" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="E50" s="30"/>
-      <c r="F50" s="30"/>
+      <c r="E50" s="40"/>
+      <c r="F50" s="40"/>
     </row>
     <row r="51" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A51" s="10" t="s">
@@ -2070,8 +2070,8 @@
       <c r="D51" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="E51" s="30"/>
-      <c r="F51" s="30"/>
+      <c r="E51" s="40"/>
+      <c r="F51" s="40"/>
     </row>
     <row r="52" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A52" s="10" t="s">
@@ -2086,16 +2086,16 @@
       <c r="D52" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="E52" s="30"/>
-      <c r="F52" s="30"/>
+      <c r="E52" s="40"/>
+      <c r="F52" s="40"/>
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="C5:F5"/>
-    <mergeCell ref="A32:D32"/>
-    <mergeCell ref="B34:C37"/>
+    <mergeCell ref="E48:F48"/>
+    <mergeCell ref="E49:F49"/>
+    <mergeCell ref="E50:F50"/>
+    <mergeCell ref="E51:F51"/>
+    <mergeCell ref="E52:F52"/>
     <mergeCell ref="A40:D40"/>
     <mergeCell ref="A25:D25"/>
     <mergeCell ref="B27:C29"/>
@@ -2103,11 +2103,11 @@
     <mergeCell ref="B31:C31"/>
     <mergeCell ref="B39:D39"/>
     <mergeCell ref="B38:C38"/>
-    <mergeCell ref="E48:F48"/>
-    <mergeCell ref="E49:F49"/>
-    <mergeCell ref="E50:F50"/>
-    <mergeCell ref="E51:F51"/>
-    <mergeCell ref="E52:F52"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="C5:F5"/>
+    <mergeCell ref="A32:D32"/>
+    <mergeCell ref="B34:C37"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="67" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
this added by last report 06-04-25
</commit_message>
<xml_diff>
--- a/Daily_Work/BL Audit Form.xlsx
+++ b/Daily_Work/BL Audit Form.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24332"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBE8260A-50AA-4FD1-865C-59BCEB1CB1C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76C310E7-9E1A-4F83-8748-4DE16F7E5F5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -233,16 +233,16 @@
     <t>লোন টু ই-লাইফ কমিউনিকেশন</t>
   </si>
   <si>
-    <t xml:space="preserve">27.03.2025 payment </t>
-  </si>
-  <si>
-    <t>26.03.2025</t>
-  </si>
-  <si>
-    <t>29.03.2025</t>
-  </si>
-  <si>
-    <t xml:space="preserve">29.03.2025 payment </t>
+    <t>05.04.2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">06.04.2025 payment </t>
+  </si>
+  <si>
+    <t>06.04.2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">07.04.2025 payment </t>
   </si>
 </sst>
 </file>
@@ -468,6 +468,12 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
@@ -497,12 +503,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2017,8 +2017,8 @@
   </sheetPr>
   <dimension ref="A1:I52"/>
   <sheetViews>
-    <sheetView topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="E41" sqref="E41"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="F35" sqref="F35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2036,7 +2036,7 @@
         <v>9</v>
       </c>
       <c r="B1" s="24" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C1" s="24"/>
       <c r="D1" s="24"/>
@@ -2047,12 +2047,12 @@
       <c r="A2" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="32" t="s">
+      <c r="B2" s="34" t="s">
         <v>59</v>
       </c>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
+      <c r="C2" s="34"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="34"/>
       <c r="F2" s="2"/>
     </row>
     <row r="3" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
@@ -2071,12 +2071,12 @@
       <c r="A4" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="B4" s="33" t="s">
+      <c r="B4" s="35" t="s">
         <v>58</v>
       </c>
-      <c r="C4" s="33"/>
-      <c r="D4" s="33"/>
-      <c r="E4" s="33"/>
+      <c r="C4" s="35"/>
+      <c r="D4" s="35"/>
+      <c r="E4" s="35"/>
       <c r="F4" s="2"/>
     </row>
     <row r="5" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
@@ -2084,12 +2084,12 @@
         <v>2</v>
       </c>
       <c r="B5" s="2"/>
-      <c r="C5" s="33" t="s">
+      <c r="C5" s="35" t="s">
         <v>57</v>
       </c>
-      <c r="D5" s="33"/>
-      <c r="E5" s="33"/>
-      <c r="F5" s="33"/>
+      <c r="D5" s="35"/>
+      <c r="E5" s="35"/>
+      <c r="F5" s="35"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="22"/>
@@ -2134,14 +2134,14 @@
         <v>46</v>
       </c>
       <c r="C9" s="2">
-        <v>38884</v>
+        <v>316088</v>
       </c>
       <c r="D9" s="2">
         <v>0.96250000000000002</v>
       </c>
       <c r="E9" s="20">
         <f>C9*D9</f>
-        <v>37425.85</v>
+        <v>304234.7</v>
       </c>
       <c r="F9" s="11"/>
     </row>
@@ -2225,14 +2225,14 @@
         <v>60</v>
       </c>
       <c r="C14" s="2">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D14" s="2">
         <v>470</v>
       </c>
       <c r="E14" s="20">
         <f t="shared" si="0"/>
-        <v>10340</v>
+        <v>9870</v>
       </c>
       <c r="F14" s="12"/>
     </row>
@@ -2261,14 +2261,14 @@
         <v>51</v>
       </c>
       <c r="C16" s="2">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="D16" s="2">
         <v>323</v>
       </c>
       <c r="E16" s="20">
         <f t="shared" si="0"/>
-        <v>2584</v>
+        <v>323</v>
       </c>
       <c r="F16" s="12"/>
     </row>
@@ -2371,7 +2371,7 @@
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
       <c r="E22" s="2">
-        <v>616863</v>
+        <v>134914</v>
       </c>
       <c r="F22" s="12"/>
     </row>
@@ -2404,15 +2404,15 @@
       <c r="F24" s="11"/>
     </row>
     <row r="25" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="34" t="s">
+      <c r="A25" s="36" t="s">
         <v>10</v>
       </c>
-      <c r="B25" s="34"/>
-      <c r="C25" s="34"/>
-      <c r="D25" s="34"/>
+      <c r="B25" s="36"/>
+      <c r="C25" s="36"/>
+      <c r="D25" s="36"/>
       <c r="E25" s="20">
         <f>SUM(E9:E24)</f>
-        <v>1180473.8500000001</v>
+        <v>962602.7</v>
       </c>
       <c r="F25" s="11"/>
     </row>
@@ -2426,10 +2426,10 @@
       <c r="A27" s="8">
         <v>17</v>
       </c>
-      <c r="B27" s="35" t="s">
+      <c r="B27" s="37" t="s">
         <v>12</v>
       </c>
-      <c r="C27" s="35"/>
+      <c r="C27" s="37"/>
       <c r="D27" s="9" t="s">
         <v>13</v>
       </c>
@@ -2440,8 +2440,8 @@
       <c r="A28" s="8">
         <v>18</v>
       </c>
-      <c r="B28" s="35"/>
-      <c r="C28" s="35"/>
+      <c r="B28" s="37"/>
+      <c r="C28" s="37"/>
       <c r="D28" s="9" t="s">
         <v>14</v>
       </c>
@@ -2452,8 +2452,8 @@
       <c r="A29" s="8">
         <v>19</v>
       </c>
-      <c r="B29" s="35"/>
-      <c r="C29" s="35"/>
+      <c r="B29" s="37"/>
+      <c r="C29" s="37"/>
       <c r="D29" s="17" t="s">
         <v>55</v>
       </c>
@@ -2464,10 +2464,10 @@
       <c r="A30" s="8">
         <v>20</v>
       </c>
-      <c r="B30" s="36" t="s">
+      <c r="B30" s="38" t="s">
         <v>16</v>
       </c>
-      <c r="C30" s="36"/>
+      <c r="C30" s="38"/>
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
       <c r="F30" s="12"/>
@@ -2476,10 +2476,10 @@
       <c r="A31" s="8">
         <v>21</v>
       </c>
-      <c r="B31" s="36" t="s">
+      <c r="B31" s="38" t="s">
         <v>15</v>
       </c>
-      <c r="C31" s="36"/>
+      <c r="C31" s="38"/>
       <c r="D31" s="30" t="s">
         <v>67</v>
       </c>
@@ -2489,15 +2489,15 @@
       <c r="F31" s="11"/>
     </row>
     <row r="32" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="34" t="s">
+      <c r="A32" s="36" t="s">
         <v>19</v>
       </c>
-      <c r="B32" s="34"/>
-      <c r="C32" s="34"/>
-      <c r="D32" s="34"/>
+      <c r="B32" s="36"/>
+      <c r="C32" s="36"/>
+      <c r="D32" s="36"/>
       <c r="E32" s="20">
         <f>E25+E31+E30+E29+E28+E27</f>
-        <v>1282473.8500000001</v>
+        <v>1064602.7</v>
       </c>
       <c r="F32" s="11"/>
       <c r="I32" t="s">
@@ -2514,26 +2514,26 @@
       <c r="A34" s="8">
         <v>22</v>
       </c>
-      <c r="B34" s="35" t="s">
+      <c r="B34" s="37" t="s">
         <v>23</v>
       </c>
-      <c r="C34" s="35"/>
+      <c r="C34" s="37"/>
       <c r="D34" s="9" t="s">
         <v>24</v>
       </c>
       <c r="E34" s="2">
-        <v>400000</v>
+        <v>204500</v>
       </c>
       <c r="F34" s="21" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="8">
         <v>23</v>
       </c>
-      <c r="B35" s="35"/>
-      <c r="C35" s="35"/>
+      <c r="B35" s="37"/>
+      <c r="C35" s="37"/>
       <c r="D35" s="9" t="s">
         <v>25</v>
       </c>
@@ -2544,8 +2544,8 @@
       <c r="A36" s="8">
         <v>24</v>
       </c>
-      <c r="B36" s="35"/>
-      <c r="C36" s="35"/>
+      <c r="B36" s="37"/>
+      <c r="C36" s="37"/>
       <c r="D36" s="9" t="s">
         <v>26</v>
       </c>
@@ -2556,8 +2556,8 @@
       <c r="A37" s="8">
         <v>25</v>
       </c>
-      <c r="B37" s="35"/>
-      <c r="C37" s="35"/>
+      <c r="B37" s="37"/>
+      <c r="C37" s="37"/>
       <c r="D37" s="25" t="s">
         <v>61</v>
       </c>
@@ -2568,37 +2568,37 @@
       <c r="A38" s="8">
         <v>26</v>
       </c>
-      <c r="B38" s="37" t="s">
+      <c r="B38" s="39" t="s">
         <v>15</v>
       </c>
-      <c r="C38" s="38"/>
+      <c r="C38" s="40"/>
       <c r="D38" s="29"/>
       <c r="E38" s="2"/>
       <c r="F38" s="11"/>
     </row>
     <row r="39" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="28"/>
-      <c r="B39" s="39" t="s">
+      <c r="B39" s="41" t="s">
         <v>62</v>
       </c>
-      <c r="C39" s="39"/>
-      <c r="D39" s="40"/>
+      <c r="C39" s="41"/>
+      <c r="D39" s="42"/>
       <c r="E39" s="26">
         <f>SUM(E34:E38)</f>
-        <v>400000</v>
+        <v>204500</v>
       </c>
       <c r="F39" s="11"/>
     </row>
     <row r="40" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A40" s="31" t="s">
+      <c r="A40" s="33" t="s">
         <v>27</v>
       </c>
-      <c r="B40" s="31"/>
-      <c r="C40" s="31"/>
-      <c r="D40" s="31"/>
+      <c r="B40" s="33"/>
+      <c r="C40" s="33"/>
+      <c r="D40" s="33"/>
       <c r="E40" s="27">
         <f>E32-E34-E35-E36-E37-E38</f>
-        <v>882473.85000000009</v>
+        <v>860102.7</v>
       </c>
       <c r="F40" s="11"/>
     </row>
@@ -2636,8 +2636,8 @@
       <c r="D48" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="E48" s="41"/>
-      <c r="F48" s="41"/>
+      <c r="E48" s="31"/>
+      <c r="F48" s="31"/>
     </row>
     <row r="49" spans="1:6" s="16" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A49" s="14" t="s">
@@ -2652,8 +2652,8 @@
       <c r="D49" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="E49" s="42"/>
-      <c r="F49" s="42"/>
+      <c r="E49" s="32"/>
+      <c r="F49" s="32"/>
     </row>
     <row r="50" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A50" s="10" t="s">
@@ -2668,8 +2668,8 @@
       <c r="D50" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="E50" s="41"/>
-      <c r="F50" s="41"/>
+      <c r="E50" s="31"/>
+      <c r="F50" s="31"/>
     </row>
     <row r="51" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A51" s="10" t="s">
@@ -2684,8 +2684,8 @@
       <c r="D51" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="E51" s="41"/>
-      <c r="F51" s="41"/>
+      <c r="E51" s="31"/>
+      <c r="F51" s="31"/>
     </row>
     <row r="52" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A52" s="10" t="s">
@@ -2700,8 +2700,727 @@
       <c r="D52" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="E52" s="41"/>
-      <c r="F52" s="41"/>
+      <c r="E52" s="31"/>
+      <c r="F52" s="31"/>
+    </row>
+  </sheetData>
+  <mergeCells count="17">
+    <mergeCell ref="A40:D40"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="C5:F5"/>
+    <mergeCell ref="A25:D25"/>
+    <mergeCell ref="B27:C29"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="A32:D32"/>
+    <mergeCell ref="B34:C37"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="B39:D39"/>
+    <mergeCell ref="E48:F48"/>
+    <mergeCell ref="E49:F49"/>
+    <mergeCell ref="E50:F50"/>
+    <mergeCell ref="E51:F51"/>
+    <mergeCell ref="E52:F52"/>
+  </mergeCells>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="66" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F90D827A-F1D2-4176-BF87-1A9A27F5C9F5}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:I52"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="F35" sqref="F35"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12" customWidth="1"/>
+    <col min="2" max="2" width="28.42578125" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" customWidth="1"/>
+    <col min="4" max="4" width="16.5703125" customWidth="1"/>
+    <col min="5" max="5" width="16.42578125" customWidth="1"/>
+    <col min="6" max="6" width="35.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="24" t="s">
+        <v>70</v>
+      </c>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+    </row>
+    <row r="2" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A2" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="34" t="s">
+        <v>59</v>
+      </c>
+      <c r="C2" s="34"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="34"/>
+      <c r="F2" s="2"/>
+    </row>
+    <row r="3" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A3" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+    </row>
+    <row r="4" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A4" s="23" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" s="35" t="s">
+        <v>58</v>
+      </c>
+      <c r="C4" s="35"/>
+      <c r="D4" s="35"/>
+      <c r="E4" s="35"/>
+      <c r="F4" s="2"/>
+    </row>
+    <row r="5" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A5" s="23" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="2"/>
+      <c r="C5" s="35" t="s">
+        <v>57</v>
+      </c>
+      <c r="D5" s="35"/>
+      <c r="E5" s="35"/>
+      <c r="F5" s="35"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="22"/>
+      <c r="B6" s="22"/>
+      <c r="C6" s="22"/>
+      <c r="D6" s="22"/>
+      <c r="E6" s="22"/>
+      <c r="F6" s="22">
+        <v>1964151517</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A7" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" s="1" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="7">
+        <v>1</v>
+      </c>
+      <c r="B9" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="C9" s="2">
+        <v>355437</v>
+      </c>
+      <c r="D9" s="2">
+        <v>0.96250000000000002</v>
+      </c>
+      <c r="E9" s="20">
+        <f>C9*D9</f>
+        <v>342108.11249999999</v>
+      </c>
+      <c r="F9" s="11"/>
+    </row>
+    <row r="10" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="7">
+        <v>2</v>
+      </c>
+      <c r="B10" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2">
+        <v>27.97</v>
+      </c>
+      <c r="E10" s="20">
+        <f t="shared" ref="E10:E21" si="0">C10*D10</f>
+        <v>0</v>
+      </c>
+      <c r="F10" s="12"/>
+    </row>
+    <row r="11" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="7">
+        <v>3</v>
+      </c>
+      <c r="B11" s="18" t="s">
+        <v>63</v>
+      </c>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2">
+        <v>27.936800000000002</v>
+      </c>
+      <c r="E11" s="20">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F11" s="12"/>
+    </row>
+    <row r="12" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="7">
+        <v>4</v>
+      </c>
+      <c r="B12" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="C12" s="2">
+        <v>4000</v>
+      </c>
+      <c r="D12" s="2">
+        <v>18.63</v>
+      </c>
+      <c r="E12" s="20">
+        <f t="shared" si="0"/>
+        <v>74520</v>
+      </c>
+      <c r="F12" s="12"/>
+    </row>
+    <row r="13" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="7">
+        <v>5</v>
+      </c>
+      <c r="B13" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="C13" s="2">
+        <v>31</v>
+      </c>
+      <c r="D13" s="2">
+        <v>241</v>
+      </c>
+      <c r="E13" s="20">
+        <f t="shared" si="0"/>
+        <v>7471</v>
+      </c>
+      <c r="F13" s="12"/>
+    </row>
+    <row r="14" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="7">
+        <v>6</v>
+      </c>
+      <c r="B14" s="19" t="s">
+        <v>60</v>
+      </c>
+      <c r="C14" s="2">
+        <v>21</v>
+      </c>
+      <c r="D14" s="2">
+        <v>470</v>
+      </c>
+      <c r="E14" s="20">
+        <f t="shared" si="0"/>
+        <v>9870</v>
+      </c>
+      <c r="F14" s="12"/>
+    </row>
+    <row r="15" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="7">
+        <v>7</v>
+      </c>
+      <c r="B15" s="19" t="s">
+        <v>50</v>
+      </c>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2">
+        <v>341</v>
+      </c>
+      <c r="E15" s="20">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F15" s="12"/>
+    </row>
+    <row r="16" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="7">
+        <v>8</v>
+      </c>
+      <c r="B16" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="C16" s="2">
+        <v>101</v>
+      </c>
+      <c r="D16" s="2">
+        <v>323</v>
+      </c>
+      <c r="E16" s="20">
+        <f t="shared" si="0"/>
+        <v>32623</v>
+      </c>
+      <c r="F16" s="12"/>
+    </row>
+    <row r="17" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="7">
+        <v>9</v>
+      </c>
+      <c r="B17" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="C17" s="2">
+        <v>72</v>
+      </c>
+      <c r="D17" s="2">
+        <v>100</v>
+      </c>
+      <c r="E17" s="20">
+        <f t="shared" si="0"/>
+        <v>7200</v>
+      </c>
+      <c r="F17" s="12"/>
+    </row>
+    <row r="18" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="7">
+        <v>10</v>
+      </c>
+      <c r="B18" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2">
+        <v>47.162500000000001</v>
+      </c>
+      <c r="E18" s="20">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F18" s="12"/>
+    </row>
+    <row r="19" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="7">
+        <v>11</v>
+      </c>
+      <c r="B19" s="19" t="s">
+        <v>64</v>
+      </c>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2">
+        <v>19.48</v>
+      </c>
+      <c r="E19" s="20">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F19" s="12"/>
+    </row>
+    <row r="20" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="7">
+        <v>12</v>
+      </c>
+      <c r="B20" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2">
+        <v>8.81</v>
+      </c>
+      <c r="E20" s="20">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F20" s="12"/>
+    </row>
+    <row r="21" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="7">
+        <v>13</v>
+      </c>
+      <c r="B21" s="19" t="s">
+        <v>66</v>
+      </c>
+      <c r="C21" s="2">
+        <v>30</v>
+      </c>
+      <c r="D21" s="2">
+        <v>470</v>
+      </c>
+      <c r="E21" s="20">
+        <f t="shared" si="0"/>
+        <v>14100</v>
+      </c>
+      <c r="F21" s="12"/>
+    </row>
+    <row r="22" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="7">
+        <v>14</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C22" s="2"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2">
+        <v>45167</v>
+      </c>
+      <c r="F22" s="12"/>
+    </row>
+    <row r="23" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="7">
+        <v>15</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C23" s="2"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2">
+        <v>15670</v>
+      </c>
+      <c r="F23" s="12"/>
+    </row>
+    <row r="24" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="7">
+        <v>16</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2">
+        <v>400000</v>
+      </c>
+      <c r="F24" s="11"/>
+    </row>
+    <row r="25" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="36" t="s">
+        <v>10</v>
+      </c>
+      <c r="B25" s="36"/>
+      <c r="C25" s="36"/>
+      <c r="D25" s="36"/>
+      <c r="E25" s="20">
+        <f>SUM(E9:E24)</f>
+        <v>948729.11250000005</v>
+      </c>
+      <c r="F25" s="11"/>
+    </row>
+    <row r="26" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F26" s="13"/>
+    </row>
+    <row r="27" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="8">
+        <v>17</v>
+      </c>
+      <c r="B27" s="37" t="s">
+        <v>12</v>
+      </c>
+      <c r="C27" s="37"/>
+      <c r="D27" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="E27" s="2"/>
+      <c r="F27" s="12"/>
+    </row>
+    <row r="28" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="8">
+        <v>18</v>
+      </c>
+      <c r="B28" s="37"/>
+      <c r="C28" s="37"/>
+      <c r="D28" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="E28" s="2"/>
+      <c r="F28" s="12"/>
+    </row>
+    <row r="29" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="8">
+        <v>19</v>
+      </c>
+      <c r="B29" s="37"/>
+      <c r="C29" s="37"/>
+      <c r="D29" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="E29" s="2"/>
+      <c r="F29" s="11"/>
+    </row>
+    <row r="30" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="8">
+        <v>20</v>
+      </c>
+      <c r="B30" s="38" t="s">
+        <v>16</v>
+      </c>
+      <c r="C30" s="38"/>
+      <c r="D30" s="2"/>
+      <c r="E30" s="2"/>
+      <c r="F30" s="12"/>
+    </row>
+    <row r="31" spans="1:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="8">
+        <v>21</v>
+      </c>
+      <c r="B31" s="38" t="s">
+        <v>15</v>
+      </c>
+      <c r="C31" s="38"/>
+      <c r="D31" s="30" t="s">
+        <v>67</v>
+      </c>
+      <c r="E31" s="2">
+        <v>102000</v>
+      </c>
+      <c r="F31" s="11"/>
+    </row>
+    <row r="32" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="36" t="s">
+        <v>19</v>
+      </c>
+      <c r="B32" s="36"/>
+      <c r="C32" s="36"/>
+      <c r="D32" s="36"/>
+      <c r="E32" s="20">
+        <f>E25+E31+E30+E29+E28+E27</f>
+        <v>1050729.1125</v>
+      </c>
+      <c r="F32" s="11"/>
+      <c r="I32" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F33" s="13"/>
+    </row>
+    <row r="34" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="8">
+        <v>22</v>
+      </c>
+      <c r="B34" s="37" t="s">
+        <v>23</v>
+      </c>
+      <c r="C34" s="37"/>
+      <c r="D34" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="E34" s="2">
+        <v>189500</v>
+      </c>
+      <c r="F34" s="21" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="8">
+        <v>23</v>
+      </c>
+      <c r="B35" s="37"/>
+      <c r="C35" s="37"/>
+      <c r="D35" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="E35" s="2"/>
+      <c r="F35" s="11"/>
+    </row>
+    <row r="36" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="8">
+        <v>24</v>
+      </c>
+      <c r="B36" s="37"/>
+      <c r="C36" s="37"/>
+      <c r="D36" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="E36" s="2"/>
+      <c r="F36" s="11"/>
+    </row>
+    <row r="37" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="8">
+        <v>25</v>
+      </c>
+      <c r="B37" s="37"/>
+      <c r="C37" s="37"/>
+      <c r="D37" s="25" t="s">
+        <v>61</v>
+      </c>
+      <c r="E37" s="2"/>
+      <c r="F37" s="11"/>
+    </row>
+    <row r="38" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="8">
+        <v>26</v>
+      </c>
+      <c r="B38" s="39" t="s">
+        <v>15</v>
+      </c>
+      <c r="C38" s="40"/>
+      <c r="D38" s="29"/>
+      <c r="E38" s="2"/>
+      <c r="F38" s="11"/>
+    </row>
+    <row r="39" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="28"/>
+      <c r="B39" s="41" t="s">
+        <v>62</v>
+      </c>
+      <c r="C39" s="41"/>
+      <c r="D39" s="42"/>
+      <c r="E39" s="26">
+        <f>SUM(E34:E38)</f>
+        <v>189500</v>
+      </c>
+      <c r="F39" s="11"/>
+    </row>
+    <row r="40" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A40" s="33" t="s">
+        <v>27</v>
+      </c>
+      <c r="B40" s="33"/>
+      <c r="C40" s="33"/>
+      <c r="D40" s="33"/>
+      <c r="E40" s="27">
+        <f>E32-E34-E35-E36-E37-E38</f>
+        <v>861229.11250000005</v>
+      </c>
+      <c r="F40" s="11"/>
+    </row>
+    <row r="44" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="B44" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D44" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="F44" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A46" s="10" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A47" s="10" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A48" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="B48" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="C48" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="D48" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="E48" s="31"/>
+      <c r="F48" s="31"/>
+    </row>
+    <row r="49" spans="1:6" s="16" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A49" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="B49" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="C49" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="D49" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="E49" s="32"/>
+      <c r="F49" s="32"/>
+    </row>
+    <row r="50" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A50" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="B50" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="C50" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="D50" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="E50" s="31"/>
+      <c r="F50" s="31"/>
+    </row>
+    <row r="51" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A51" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="B51" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="C51" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="D51" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="E51" s="31"/>
+      <c r="F51" s="31"/>
+    </row>
+    <row r="52" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A52" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="B52" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="C52" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="D52" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="E52" s="31"/>
+      <c r="F52" s="31"/>
     </row>
   </sheetData>
   <mergeCells count="17">
@@ -2727,723 +3446,4 @@
   <pageSetup paperSize="9" scale="66" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F90D827A-F1D2-4176-BF87-1A9A27F5C9F5}">
-  <sheetPr>
-    <pageSetUpPr fitToPage="1"/>
-  </sheetPr>
-  <dimension ref="A1:I52"/>
-  <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="F35" sqref="F35"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="12" customWidth="1"/>
-    <col min="2" max="2" width="28.42578125" customWidth="1"/>
-    <col min="3" max="3" width="13.5703125" customWidth="1"/>
-    <col min="4" max="4" width="16.5703125" customWidth="1"/>
-    <col min="5" max="5" width="16.42578125" customWidth="1"/>
-    <col min="6" max="6" width="35.28515625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="23" t="s">
-        <v>9</v>
-      </c>
-      <c r="B1" s="24" t="s">
-        <v>70</v>
-      </c>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-    </row>
-    <row r="2" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A2" s="23" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="32" t="s">
-        <v>59</v>
-      </c>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="2"/>
-    </row>
-    <row r="3" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A3" s="23" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-    </row>
-    <row r="4" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A4" s="23" t="s">
-        <v>28</v>
-      </c>
-      <c r="B4" s="33" t="s">
-        <v>58</v>
-      </c>
-      <c r="C4" s="33"/>
-      <c r="D4" s="33"/>
-      <c r="E4" s="33"/>
-      <c r="F4" s="2"/>
-    </row>
-    <row r="5" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A5" s="23" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" s="2"/>
-      <c r="C5" s="33" t="s">
-        <v>57</v>
-      </c>
-      <c r="D5" s="33"/>
-      <c r="E5" s="33"/>
-      <c r="F5" s="33"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="22"/>
-      <c r="B6" s="22"/>
-      <c r="C6" s="22"/>
-      <c r="D6" s="22"/>
-      <c r="E6" s="22"/>
-      <c r="F6" s="22">
-        <v>1964151517</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A7" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" s="1" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="E8" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="F8" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="7">
-        <v>1</v>
-      </c>
-      <c r="B9" s="18" t="s">
-        <v>46</v>
-      </c>
-      <c r="C9" s="2">
-        <v>450388</v>
-      </c>
-      <c r="D9" s="2">
-        <v>0.96250000000000002</v>
-      </c>
-      <c r="E9" s="20">
-        <f>C9*D9</f>
-        <v>433498.45</v>
-      </c>
-      <c r="F9" s="11"/>
-    </row>
-    <row r="10" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="7">
-        <v>2</v>
-      </c>
-      <c r="B10" s="18" t="s">
-        <v>47</v>
-      </c>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2">
-        <v>27.97</v>
-      </c>
-      <c r="E10" s="20">
-        <f t="shared" ref="E10:E21" si="0">C10*D10</f>
-        <v>0</v>
-      </c>
-      <c r="F10" s="12"/>
-    </row>
-    <row r="11" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="7">
-        <v>3</v>
-      </c>
-      <c r="B11" s="18" t="s">
-        <v>63</v>
-      </c>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2">
-        <v>27.936800000000002</v>
-      </c>
-      <c r="E11" s="20">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F11" s="12"/>
-    </row>
-    <row r="12" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="7">
-        <v>4</v>
-      </c>
-      <c r="B12" s="19" t="s">
-        <v>48</v>
-      </c>
-      <c r="C12" s="2">
-        <v>4000</v>
-      </c>
-      <c r="D12" s="2">
-        <v>18.63</v>
-      </c>
-      <c r="E12" s="20">
-        <f t="shared" si="0"/>
-        <v>74520</v>
-      </c>
-      <c r="F12" s="12"/>
-    </row>
-    <row r="13" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="7">
-        <v>5</v>
-      </c>
-      <c r="B13" s="19" t="s">
-        <v>49</v>
-      </c>
-      <c r="C13" s="2">
-        <v>31</v>
-      </c>
-      <c r="D13" s="2">
-        <v>241</v>
-      </c>
-      <c r="E13" s="20">
-        <f t="shared" si="0"/>
-        <v>7471</v>
-      </c>
-      <c r="F13" s="12"/>
-    </row>
-    <row r="14" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="7">
-        <v>6</v>
-      </c>
-      <c r="B14" s="19" t="s">
-        <v>60</v>
-      </c>
-      <c r="C14" s="2">
-        <v>21</v>
-      </c>
-      <c r="D14" s="2">
-        <v>470</v>
-      </c>
-      <c r="E14" s="20">
-        <f t="shared" si="0"/>
-        <v>9870</v>
-      </c>
-      <c r="F14" s="12"/>
-    </row>
-    <row r="15" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="7">
-        <v>7</v>
-      </c>
-      <c r="B15" s="19" t="s">
-        <v>50</v>
-      </c>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2">
-        <v>341</v>
-      </c>
-      <c r="E15" s="20">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F15" s="12"/>
-    </row>
-    <row r="16" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="7">
-        <v>8</v>
-      </c>
-      <c r="B16" s="19" t="s">
-        <v>51</v>
-      </c>
-      <c r="C16" s="2">
-        <v>1</v>
-      </c>
-      <c r="D16" s="2">
-        <v>323</v>
-      </c>
-      <c r="E16" s="20">
-        <f t="shared" si="0"/>
-        <v>323</v>
-      </c>
-      <c r="F16" s="12"/>
-    </row>
-    <row r="17" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="7">
-        <v>9</v>
-      </c>
-      <c r="B17" s="19" t="s">
-        <v>52</v>
-      </c>
-      <c r="C17" s="2">
-        <v>72</v>
-      </c>
-      <c r="D17" s="2">
-        <v>100</v>
-      </c>
-      <c r="E17" s="20">
-        <f t="shared" si="0"/>
-        <v>7200</v>
-      </c>
-      <c r="F17" s="12"/>
-    </row>
-    <row r="18" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="7">
-        <v>10</v>
-      </c>
-      <c r="B18" s="19" t="s">
-        <v>53</v>
-      </c>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2">
-        <v>47.162500000000001</v>
-      </c>
-      <c r="E18" s="20">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F18" s="12"/>
-    </row>
-    <row r="19" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="7">
-        <v>11</v>
-      </c>
-      <c r="B19" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2">
-        <v>19.48</v>
-      </c>
-      <c r="E19" s="20">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F19" s="12"/>
-    </row>
-    <row r="20" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="7">
-        <v>12</v>
-      </c>
-      <c r="B20" s="19" t="s">
-        <v>54</v>
-      </c>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2">
-        <v>8.81</v>
-      </c>
-      <c r="E20" s="20">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F20" s="12"/>
-    </row>
-    <row r="21" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="7">
-        <v>13</v>
-      </c>
-      <c r="B21" s="19" t="s">
-        <v>66</v>
-      </c>
-      <c r="C21" s="2">
-        <v>20</v>
-      </c>
-      <c r="D21" s="2">
-        <v>470</v>
-      </c>
-      <c r="E21" s="20">
-        <f t="shared" si="0"/>
-        <v>9400</v>
-      </c>
-      <c r="F21" s="12"/>
-    </row>
-    <row r="22" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="7">
-        <v>14</v>
-      </c>
-      <c r="B22" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
-      <c r="E22" s="2">
-        <v>6967</v>
-      </c>
-      <c r="F22" s="12"/>
-    </row>
-    <row r="23" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="7">
-        <v>15</v>
-      </c>
-      <c r="B23" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="C23" s="2"/>
-      <c r="D23" s="2"/>
-      <c r="E23" s="2">
-        <v>14670</v>
-      </c>
-      <c r="F23" s="12"/>
-    </row>
-    <row r="24" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="7">
-        <v>16</v>
-      </c>
-      <c r="B24" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C24" s="2"/>
-      <c r="D24" s="2"/>
-      <c r="E24" s="2">
-        <v>400000</v>
-      </c>
-      <c r="F24" s="11"/>
-    </row>
-    <row r="25" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="34" t="s">
-        <v>10</v>
-      </c>
-      <c r="B25" s="34"/>
-      <c r="C25" s="34"/>
-      <c r="D25" s="34"/>
-      <c r="E25" s="20">
-        <f>SUM(E9:E24)</f>
-        <v>963919.45</v>
-      </c>
-      <c r="F25" s="11"/>
-    </row>
-    <row r="26" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="F26" s="13"/>
-    </row>
-    <row r="27" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="8">
-        <v>17</v>
-      </c>
-      <c r="B27" s="35" t="s">
-        <v>12</v>
-      </c>
-      <c r="C27" s="35"/>
-      <c r="D27" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="E27" s="2"/>
-      <c r="F27" s="12"/>
-    </row>
-    <row r="28" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="8">
-        <v>18</v>
-      </c>
-      <c r="B28" s="35"/>
-      <c r="C28" s="35"/>
-      <c r="D28" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="E28" s="2"/>
-      <c r="F28" s="12"/>
-    </row>
-    <row r="29" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="8">
-        <v>19</v>
-      </c>
-      <c r="B29" s="35"/>
-      <c r="C29" s="35"/>
-      <c r="D29" s="17" t="s">
-        <v>55</v>
-      </c>
-      <c r="E29" s="2"/>
-      <c r="F29" s="11"/>
-    </row>
-    <row r="30" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="8">
-        <v>20</v>
-      </c>
-      <c r="B30" s="36" t="s">
-        <v>16</v>
-      </c>
-      <c r="C30" s="36"/>
-      <c r="D30" s="2"/>
-      <c r="E30" s="2"/>
-      <c r="F30" s="12"/>
-    </row>
-    <row r="31" spans="1:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="8">
-        <v>21</v>
-      </c>
-      <c r="B31" s="36" t="s">
-        <v>15</v>
-      </c>
-      <c r="C31" s="36"/>
-      <c r="D31" s="30" t="s">
-        <v>67</v>
-      </c>
-      <c r="E31" s="2">
-        <v>102000</v>
-      </c>
-      <c r="F31" s="11"/>
-    </row>
-    <row r="32" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="34" t="s">
-        <v>19</v>
-      </c>
-      <c r="B32" s="34"/>
-      <c r="C32" s="34"/>
-      <c r="D32" s="34"/>
-      <c r="E32" s="20">
-        <f>E25+E31+E30+E29+E28+E27</f>
-        <v>1065919.45</v>
-      </c>
-      <c r="F32" s="11"/>
-      <c r="I32" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="F33" s="13"/>
-    </row>
-    <row r="34" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="8">
-        <v>22</v>
-      </c>
-      <c r="B34" s="35" t="s">
-        <v>23</v>
-      </c>
-      <c r="C34" s="35"/>
-      <c r="D34" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="E34" s="2">
-        <v>204500</v>
-      </c>
-      <c r="F34" s="21" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="8">
-        <v>23</v>
-      </c>
-      <c r="B35" s="35"/>
-      <c r="C35" s="35"/>
-      <c r="D35" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="E35" s="2"/>
-      <c r="F35" s="11"/>
-    </row>
-    <row r="36" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="8">
-        <v>24</v>
-      </c>
-      <c r="B36" s="35"/>
-      <c r="C36" s="35"/>
-      <c r="D36" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="E36" s="2"/>
-      <c r="F36" s="11"/>
-    </row>
-    <row r="37" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="8">
-        <v>25</v>
-      </c>
-      <c r="B37" s="35"/>
-      <c r="C37" s="35"/>
-      <c r="D37" s="25" t="s">
-        <v>61</v>
-      </c>
-      <c r="E37" s="2"/>
-      <c r="F37" s="11"/>
-    </row>
-    <row r="38" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="8">
-        <v>26</v>
-      </c>
-      <c r="B38" s="37" t="s">
-        <v>15</v>
-      </c>
-      <c r="C38" s="38"/>
-      <c r="D38" s="29"/>
-      <c r="E38" s="2"/>
-      <c r="F38" s="11"/>
-    </row>
-    <row r="39" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="28"/>
-      <c r="B39" s="39" t="s">
-        <v>62</v>
-      </c>
-      <c r="C39" s="39"/>
-      <c r="D39" s="40"/>
-      <c r="E39" s="26">
-        <f>SUM(E34:E38)</f>
-        <v>204500</v>
-      </c>
-      <c r="F39" s="11"/>
-    </row>
-    <row r="40" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A40" s="31" t="s">
-        <v>27</v>
-      </c>
-      <c r="B40" s="31"/>
-      <c r="C40" s="31"/>
-      <c r="D40" s="31"/>
-      <c r="E40" s="27">
-        <f>E32-E34-E35-E36-E37-E38</f>
-        <v>861419.45</v>
-      </c>
-      <c r="F40" s="11"/>
-    </row>
-    <row r="44" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="B44" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="D44" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="F44" s="4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A46" s="10" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A47" s="10" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A48" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="B48" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="C48" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="D48" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="E48" s="41"/>
-      <c r="F48" s="41"/>
-    </row>
-    <row r="49" spans="1:6" s="16" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A49" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="B49" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="C49" s="14" t="s">
-        <v>35</v>
-      </c>
-      <c r="D49" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="E49" s="42"/>
-      <c r="F49" s="42"/>
-    </row>
-    <row r="50" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A50" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="B50" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="C50" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="D50" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="E50" s="41"/>
-      <c r="F50" s="41"/>
-    </row>
-    <row r="51" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A51" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="B51" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="C51" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="D51" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="E51" s="41"/>
-      <c r="F51" s="41"/>
-    </row>
-    <row r="52" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A52" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="B52" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="C52" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="D52" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="E52" s="41"/>
-      <c r="F52" s="41"/>
-    </row>
-  </sheetData>
-  <mergeCells count="17">
-    <mergeCell ref="A40:D40"/>
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="C5:F5"/>
-    <mergeCell ref="A25:D25"/>
-    <mergeCell ref="B27:C29"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="A32:D32"/>
-    <mergeCell ref="B34:C37"/>
-    <mergeCell ref="B38:C38"/>
-    <mergeCell ref="B39:D39"/>
-    <mergeCell ref="E48:F48"/>
-    <mergeCell ref="E49:F49"/>
-    <mergeCell ref="E50:F50"/>
-    <mergeCell ref="E51:F51"/>
-    <mergeCell ref="E52:F52"/>
-  </mergeCells>
-  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="66" orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
this added by last report 14-04-25
</commit_message>
<xml_diff>
--- a/Daily_Work/BL Audit Form.xlsx
+++ b/Daily_Work/BL Audit Form.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24332"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76C310E7-9E1A-4F83-8748-4DE16F7E5F5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B5F4966-CA56-4A90-BB3F-90630F854259}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -233,16 +233,16 @@
     <t>লোন টু ই-লাইফ কমিউনিকেশন</t>
   </si>
   <si>
-    <t>05.04.2025</t>
-  </si>
-  <si>
-    <t xml:space="preserve">06.04.2025 payment </t>
-  </si>
-  <si>
-    <t>06.04.2025</t>
-  </si>
-  <si>
-    <t xml:space="preserve">07.04.2025 payment </t>
+    <t xml:space="preserve">13.04.2025 payment </t>
+  </si>
+  <si>
+    <t>12.04.2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15.04.2025 payment </t>
+  </si>
+  <si>
+    <t>14.04.2025</t>
   </si>
 </sst>
 </file>
@@ -1126,7 +1126,7 @@
         <xdr:cNvPr id="2" name="Rounded Rectangle 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B09027A3-9978-4EE2-A803-D663E3FB521F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{62F528D9-2D33-4892-9D27-C47D524B02A7}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1184,7 +1184,7 @@
         <xdr:cNvPr id="3" name="Rounded Rectangle 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5F2712D9-D634-4A5D-B95F-232D7C30497E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{69AF0B0B-A8DC-4367-8FE8-908833589A66}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1242,7 +1242,7 @@
         <xdr:cNvPr id="4" name="Rounded Rectangle 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{95073152-3EB4-4F48-A933-347668319F55}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5173871A-EF32-4710-9EE1-C7B54363FE49}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1300,7 +1300,7 @@
         <xdr:cNvPr id="5" name="Rounded Rectangle 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{35A6D30F-C3C2-4473-AA87-CAE5EDD1F34A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DB6C50E7-54C9-46F5-8DA4-20D8429AE794}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1358,7 +1358,7 @@
         <xdr:cNvPr id="6" name="Rounded Rectangle 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{976DCAC9-9DEB-49F4-8A09-D94205F49A4E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D08A3819-2396-409A-BB69-AA672CCAD7A7}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1416,7 +1416,7 @@
         <xdr:cNvPr id="7" name="Rounded Rectangle 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3C2C89DF-BE97-4B59-AABB-788A54866BC3}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{66DB5C65-8EF4-487A-A521-E3D9005D36F6}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1474,7 +1474,7 @@
         <xdr:cNvPr id="8" name="Rounded Rectangle 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BD3FD15C-AF63-49B9-88F5-E0D5DCDF2BC6}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7AE2188E-88B9-4A47-BF90-19945C9D4FD2}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1532,7 +1532,7 @@
         <xdr:cNvPr id="9" name="Rounded Rectangle 8">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B6F81CDE-70D2-4A7B-8A39-9B8D8E5B9390}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4AB7AEC2-1F2E-462E-A17D-827DF4A4F33C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1590,7 +1590,7 @@
         <xdr:cNvPr id="10" name="Rounded Rectangle 9">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{34064273-6382-478C-9DEA-F2E5EDB624A8}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0CA754C1-2658-4444-9DDD-055B1FE91097}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1648,7 +1648,7 @@
         <xdr:cNvPr id="11" name="Rounded Rectangle 10">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{13BF4D62-A569-457F-93B4-C97413BCEFB6}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A24CEB03-6A42-4B37-8EDE-69F865913F24}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2017,8 +2017,8 @@
   </sheetPr>
   <dimension ref="A1:I52"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="F35" sqref="F35"/>
+    <sheetView topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2036,7 +2036,7 @@
         <v>9</v>
       </c>
       <c r="B1" s="24" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C1" s="24"/>
       <c r="D1" s="24"/>
@@ -2134,14 +2134,14 @@
         <v>46</v>
       </c>
       <c r="C9" s="2">
-        <v>316088</v>
+        <v>347259</v>
       </c>
       <c r="D9" s="2">
         <v>0.96250000000000002</v>
       </c>
       <c r="E9" s="20">
         <f>C9*D9</f>
-        <v>304234.7</v>
+        <v>334236.78750000003</v>
       </c>
       <c r="F9" s="11"/>
     </row>
@@ -2152,13 +2152,15 @@
       <c r="B10" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="C10" s="2"/>
+      <c r="C10" s="2">
+        <v>390</v>
+      </c>
       <c r="D10" s="2">
         <v>27.97</v>
       </c>
       <c r="E10" s="20">
         <f t="shared" ref="E10:E21" si="0">C10*D10</f>
-        <v>0</v>
+        <v>10908.3</v>
       </c>
       <c r="F10" s="12"/>
     </row>
@@ -2187,14 +2189,14 @@
         <v>48</v>
       </c>
       <c r="C12" s="2">
-        <v>4000</v>
+        <v>680</v>
       </c>
       <c r="D12" s="2">
         <v>18.63</v>
       </c>
       <c r="E12" s="20">
         <f t="shared" si="0"/>
-        <v>74520</v>
+        <v>12668.4</v>
       </c>
       <c r="F12" s="12"/>
     </row>
@@ -2225,14 +2227,14 @@
         <v>60</v>
       </c>
       <c r="C14" s="2">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="D14" s="2">
         <v>470</v>
       </c>
       <c r="E14" s="20">
         <f t="shared" si="0"/>
-        <v>9870</v>
+        <v>3760</v>
       </c>
       <c r="F14" s="12"/>
     </row>
@@ -2261,14 +2263,14 @@
         <v>51</v>
       </c>
       <c r="C16" s="2">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="D16" s="2">
         <v>323</v>
       </c>
       <c r="E16" s="20">
         <f t="shared" si="0"/>
-        <v>323</v>
+        <v>4845</v>
       </c>
       <c r="F16" s="12"/>
     </row>
@@ -2280,14 +2282,14 @@
         <v>52</v>
       </c>
       <c r="C17" s="2">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="D17" s="2">
         <v>100</v>
       </c>
       <c r="E17" s="20">
         <f t="shared" si="0"/>
-        <v>7200</v>
+        <v>6900</v>
       </c>
       <c r="F17" s="12"/>
     </row>
@@ -2350,14 +2352,14 @@
         <v>66</v>
       </c>
       <c r="C21" s="2">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="D21" s="2">
         <v>470</v>
       </c>
       <c r="E21" s="20">
         <f t="shared" si="0"/>
-        <v>9400</v>
+        <v>14100</v>
       </c>
       <c r="F21" s="12"/>
     </row>
@@ -2371,7 +2373,7 @@
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
       <c r="E22" s="2">
-        <v>134914</v>
+        <v>231506</v>
       </c>
       <c r="F22" s="12"/>
     </row>
@@ -2385,7 +2387,7 @@
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
       <c r="E23" s="2">
-        <v>14670</v>
+        <v>6520</v>
       </c>
       <c r="F23" s="12"/>
     </row>
@@ -2412,7 +2414,7 @@
       <c r="D25" s="36"/>
       <c r="E25" s="20">
         <f>SUM(E9:E24)</f>
-        <v>962602.7</v>
+        <v>1032915.4875</v>
       </c>
       <c r="F25" s="11"/>
     </row>
@@ -2497,7 +2499,7 @@
       <c r="D32" s="36"/>
       <c r="E32" s="20">
         <f>E25+E31+E30+E29+E28+E27</f>
-        <v>1064602.7</v>
+        <v>1134915.4875</v>
       </c>
       <c r="F32" s="11"/>
       <c r="I32" t="s">
@@ -2522,10 +2524,10 @@
         <v>24</v>
       </c>
       <c r="E34" s="2">
-        <v>204500</v>
+        <v>272000</v>
       </c>
       <c r="F34" s="21" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -2585,7 +2587,7 @@
       <c r="D39" s="42"/>
       <c r="E39" s="26">
         <f>SUM(E34:E38)</f>
-        <v>204500</v>
+        <v>272000</v>
       </c>
       <c r="F39" s="11"/>
     </row>
@@ -2598,7 +2600,7 @@
       <c r="D40" s="33"/>
       <c r="E40" s="27">
         <f>E32-E34-E35-E36-E37-E38</f>
-        <v>860102.7</v>
+        <v>862915.48750000005</v>
       </c>
       <c r="F40" s="11"/>
     </row>
@@ -2730,14 +2732,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F90D827A-F1D2-4176-BF87-1A9A27F5C9F5}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FE971A6-2634-4F84-9496-071AD9523EF2}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:I52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="F35" sqref="F35"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2755,7 +2757,7 @@
         <v>9</v>
       </c>
       <c r="B1" s="24" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C1" s="24"/>
       <c r="D1" s="24"/>
@@ -2853,14 +2855,14 @@
         <v>46</v>
       </c>
       <c r="C9" s="2">
-        <v>355437</v>
+        <v>363645</v>
       </c>
       <c r="D9" s="2">
         <v>0.96250000000000002</v>
       </c>
       <c r="E9" s="20">
         <f>C9*D9</f>
-        <v>342108.11249999999</v>
+        <v>350008.3125</v>
       </c>
       <c r="F9" s="11"/>
     </row>
@@ -2871,13 +2873,15 @@
       <c r="B10" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="C10" s="2"/>
+      <c r="C10" s="2">
+        <v>40</v>
+      </c>
       <c r="D10" s="2">
         <v>27.97</v>
       </c>
       <c r="E10" s="20">
         <f t="shared" ref="E10:E21" si="0">C10*D10</f>
-        <v>0</v>
+        <v>1118.8</v>
       </c>
       <c r="F10" s="12"/>
     </row>
@@ -2905,15 +2909,13 @@
       <c r="B12" s="19" t="s">
         <v>48</v>
       </c>
-      <c r="C12" s="2">
-        <v>4000</v>
-      </c>
+      <c r="C12" s="2"/>
       <c r="D12" s="2">
         <v>18.63</v>
       </c>
       <c r="E12" s="20">
         <f t="shared" si="0"/>
-        <v>74520</v>
+        <v>0</v>
       </c>
       <c r="F12" s="12"/>
     </row>
@@ -2944,14 +2946,14 @@
         <v>60</v>
       </c>
       <c r="C14" s="2">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="D14" s="2">
         <v>470</v>
       </c>
       <c r="E14" s="20">
         <f t="shared" si="0"/>
-        <v>9870</v>
+        <v>3760</v>
       </c>
       <c r="F14" s="12"/>
     </row>
@@ -2980,14 +2982,14 @@
         <v>51</v>
       </c>
       <c r="C16" s="2">
-        <v>101</v>
+        <v>2</v>
       </c>
       <c r="D16" s="2">
         <v>323</v>
       </c>
       <c r="E16" s="20">
         <f t="shared" si="0"/>
-        <v>32623</v>
+        <v>646</v>
       </c>
       <c r="F16" s="12"/>
     </row>
@@ -2999,14 +3001,14 @@
         <v>52</v>
       </c>
       <c r="C17" s="2">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="D17" s="2">
         <v>100</v>
       </c>
       <c r="E17" s="20">
         <f t="shared" si="0"/>
-        <v>7200</v>
+        <v>6800</v>
       </c>
       <c r="F17" s="12"/>
     </row>
@@ -3090,7 +3092,7 @@
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
       <c r="E22" s="2">
-        <v>45167</v>
+        <v>190088</v>
       </c>
       <c r="F22" s="12"/>
     </row>
@@ -3104,7 +3106,7 @@
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
       <c r="E23" s="2">
-        <v>15670</v>
+        <v>6530</v>
       </c>
       <c r="F23" s="12"/>
     </row>
@@ -3131,7 +3133,7 @@
       <c r="D25" s="36"/>
       <c r="E25" s="20">
         <f>SUM(E9:E24)</f>
-        <v>948729.11250000005</v>
+        <v>980522.11250000005</v>
       </c>
       <c r="F25" s="11"/>
     </row>
@@ -3216,7 +3218,7 @@
       <c r="D32" s="36"/>
       <c r="E32" s="20">
         <f>E25+E31+E30+E29+E28+E27</f>
-        <v>1050729.1125</v>
+        <v>1082522.1125</v>
       </c>
       <c r="F32" s="11"/>
       <c r="I32" t="s">
@@ -3241,10 +3243,10 @@
         <v>24</v>
       </c>
       <c r="E34" s="2">
-        <v>189500</v>
+        <v>188425</v>
       </c>
       <c r="F34" s="21" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -3304,7 +3306,7 @@
       <c r="D39" s="42"/>
       <c r="E39" s="26">
         <f>SUM(E34:E38)</f>
-        <v>189500</v>
+        <v>188425</v>
       </c>
       <c r="F39" s="11"/>
     </row>
@@ -3317,7 +3319,7 @@
       <c r="D40" s="33"/>
       <c r="E40" s="27">
         <f>E32-E34-E35-E36-E37-E38</f>
-        <v>861229.11250000005</v>
+        <v>894097.11250000005</v>
       </c>
       <c r="F40" s="11"/>
     </row>
@@ -3424,11 +3426,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="E48:F48"/>
-    <mergeCell ref="E49:F49"/>
-    <mergeCell ref="E50:F50"/>
-    <mergeCell ref="E51:F51"/>
-    <mergeCell ref="E52:F52"/>
     <mergeCell ref="A40:D40"/>
     <mergeCell ref="B2:E2"/>
     <mergeCell ref="B4:E4"/>
@@ -3441,6 +3438,11 @@
     <mergeCell ref="B34:C37"/>
     <mergeCell ref="B38:C38"/>
     <mergeCell ref="B39:D39"/>
+    <mergeCell ref="E48:F48"/>
+    <mergeCell ref="E49:F49"/>
+    <mergeCell ref="E50:F50"/>
+    <mergeCell ref="E51:F51"/>
+    <mergeCell ref="E52:F52"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="66" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
this added by last report for  mangComm in life
</commit_message>
<xml_diff>
--- a/Daily_Work/BL Audit Form.xlsx
+++ b/Daily_Work/BL Audit Form.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24332"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E4659AF-76F9-49D9-BE1C-1C0409E4274D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58A35EFC-AED6-4B7B-85F2-68DCD172BA17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -464,41 +464,41 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1428,8 +1428,8 @@
   </sheetPr>
   <dimension ref="A1:I52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="F35" sqref="F35"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1458,12 +1458,12 @@
       <c r="A2" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="34" t="s">
+      <c r="B2" s="32" t="s">
         <v>59</v>
       </c>
-      <c r="C2" s="34"/>
-      <c r="D2" s="34"/>
-      <c r="E2" s="34"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
       <c r="F2" s="2"/>
     </row>
     <row r="3" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
@@ -1482,12 +1482,12 @@
       <c r="A4" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="B4" s="35" t="s">
+      <c r="B4" s="33" t="s">
         <v>58</v>
       </c>
-      <c r="C4" s="35"/>
-      <c r="D4" s="35"/>
-      <c r="E4" s="35"/>
+      <c r="C4" s="33"/>
+      <c r="D4" s="33"/>
+      <c r="E4" s="33"/>
       <c r="F4" s="2"/>
     </row>
     <row r="5" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
@@ -1495,12 +1495,12 @@
         <v>2</v>
       </c>
       <c r="B5" s="2"/>
-      <c r="C5" s="35" t="s">
+      <c r="C5" s="33" t="s">
         <v>57</v>
       </c>
-      <c r="D5" s="35"/>
-      <c r="E5" s="35"/>
-      <c r="F5" s="35"/>
+      <c r="D5" s="33"/>
+      <c r="E5" s="33"/>
+      <c r="F5" s="33"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="22"/>
@@ -1774,7 +1774,7 @@
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
       <c r="E22" s="2">
-        <v>85086</v>
+        <v>78716</v>
       </c>
       <c r="F22" s="12"/>
     </row>
@@ -1807,15 +1807,15 @@
       <c r="F24" s="11"/>
     </row>
     <row r="25" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="36" t="s">
+      <c r="A25" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="B25" s="36"/>
-      <c r="C25" s="36"/>
-      <c r="D25" s="36"/>
+      <c r="B25" s="34"/>
+      <c r="C25" s="34"/>
+      <c r="D25" s="34"/>
       <c r="E25" s="20">
         <f>SUM(E9:E24)</f>
-        <v>506018</v>
+        <v>499648</v>
       </c>
       <c r="F25" s="11"/>
     </row>
@@ -1829,10 +1829,10 @@
       <c r="A27" s="8">
         <v>17</v>
       </c>
-      <c r="B27" s="37" t="s">
+      <c r="B27" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="C27" s="37"/>
+      <c r="C27" s="35"/>
       <c r="D27" s="9" t="s">
         <v>13</v>
       </c>
@@ -1843,8 +1843,8 @@
       <c r="A28" s="8">
         <v>18</v>
       </c>
-      <c r="B28" s="37"/>
-      <c r="C28" s="37"/>
+      <c r="B28" s="35"/>
+      <c r="C28" s="35"/>
       <c r="D28" s="9" t="s">
         <v>14</v>
       </c>
@@ -1855,8 +1855,8 @@
       <c r="A29" s="8">
         <v>19</v>
       </c>
-      <c r="B29" s="37"/>
-      <c r="C29" s="37"/>
+      <c r="B29" s="35"/>
+      <c r="C29" s="35"/>
       <c r="D29" s="17" t="s">
         <v>55</v>
       </c>
@@ -1867,10 +1867,10 @@
       <c r="A30" s="8">
         <v>20</v>
       </c>
-      <c r="B30" s="38" t="s">
+      <c r="B30" s="36" t="s">
         <v>16</v>
       </c>
-      <c r="C30" s="38"/>
+      <c r="C30" s="36"/>
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
       <c r="F30" s="12"/>
@@ -1879,10 +1879,10 @@
       <c r="A31" s="8">
         <v>21</v>
       </c>
-      <c r="B31" s="38" t="s">
+      <c r="B31" s="36" t="s">
         <v>15</v>
       </c>
-      <c r="C31" s="38"/>
+      <c r="C31" s="36"/>
       <c r="D31" s="30" t="s">
         <v>68</v>
       </c>
@@ -1893,15 +1893,15 @@
       <c r="F31" s="11"/>
     </row>
     <row r="32" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="36" t="s">
+      <c r="A32" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="B32" s="36"/>
-      <c r="C32" s="36"/>
-      <c r="D32" s="36"/>
+      <c r="B32" s="34"/>
+      <c r="C32" s="34"/>
+      <c r="D32" s="34"/>
       <c r="E32" s="20">
         <f>E25+E31+E30+E29+E28+E27</f>
-        <v>864018</v>
+        <v>857648</v>
       </c>
       <c r="F32" s="11"/>
       <c r="I32" t="s">
@@ -1918,10 +1918,10 @@
       <c r="A34" s="8">
         <v>22</v>
       </c>
-      <c r="B34" s="37" t="s">
+      <c r="B34" s="35" t="s">
         <v>23</v>
       </c>
-      <c r="C34" s="37"/>
+      <c r="C34" s="35"/>
       <c r="D34" s="9" t="s">
         <v>24</v>
       </c>
@@ -1934,8 +1934,8 @@
       <c r="A35" s="8">
         <v>23</v>
       </c>
-      <c r="B35" s="37"/>
-      <c r="C35" s="37"/>
+      <c r="B35" s="35"/>
+      <c r="C35" s="35"/>
       <c r="D35" s="9" t="s">
         <v>25</v>
       </c>
@@ -1948,8 +1948,8 @@
       <c r="A36" s="8">
         <v>24</v>
       </c>
-      <c r="B36" s="37"/>
-      <c r="C36" s="37"/>
+      <c r="B36" s="35"/>
+      <c r="C36" s="35"/>
       <c r="D36" s="9" t="s">
         <v>26</v>
       </c>
@@ -1960,8 +1960,8 @@
       <c r="A37" s="8">
         <v>25</v>
       </c>
-      <c r="B37" s="37"/>
-      <c r="C37" s="37"/>
+      <c r="B37" s="35"/>
+      <c r="C37" s="35"/>
       <c r="D37" s="25" t="s">
         <v>61</v>
       </c>
@@ -1972,21 +1972,21 @@
       <c r="A38" s="8">
         <v>26</v>
       </c>
-      <c r="B38" s="39" t="s">
+      <c r="B38" s="37" t="s">
         <v>15</v>
       </c>
-      <c r="C38" s="40"/>
+      <c r="C38" s="38"/>
       <c r="D38" s="29"/>
       <c r="E38" s="2"/>
       <c r="F38" s="11"/>
     </row>
     <row r="39" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="28"/>
-      <c r="B39" s="41" t="s">
+      <c r="B39" s="39" t="s">
         <v>62</v>
       </c>
-      <c r="C39" s="41"/>
-      <c r="D39" s="42"/>
+      <c r="C39" s="39"/>
+      <c r="D39" s="40"/>
       <c r="E39" s="26">
         <f>SUM(E34:E38)</f>
         <v>0</v>
@@ -1994,15 +1994,15 @@
       <c r="F39" s="11"/>
     </row>
     <row r="40" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A40" s="33" t="s">
+      <c r="A40" s="31" t="s">
         <v>27</v>
       </c>
-      <c r="B40" s="33"/>
-      <c r="C40" s="33"/>
-      <c r="D40" s="33"/>
+      <c r="B40" s="31"/>
+      <c r="C40" s="31"/>
+      <c r="D40" s="31"/>
       <c r="E40" s="27">
         <f>E32-E34-E35-E36-E37-E38</f>
-        <v>864018</v>
+        <v>857648</v>
       </c>
       <c r="F40" s="11"/>
     </row>
@@ -2040,8 +2040,8 @@
       <c r="D48" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="E48" s="31"/>
-      <c r="F48" s="31"/>
+      <c r="E48" s="41"/>
+      <c r="F48" s="41"/>
     </row>
     <row r="49" spans="1:6" s="16" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A49" s="14" t="s">
@@ -2056,8 +2056,8 @@
       <c r="D49" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="E49" s="32"/>
-      <c r="F49" s="32"/>
+      <c r="E49" s="42"/>
+      <c r="F49" s="42"/>
     </row>
     <row r="50" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A50" s="10" t="s">
@@ -2072,8 +2072,8 @@
       <c r="D50" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="E50" s="31"/>
-      <c r="F50" s="31"/>
+      <c r="E50" s="41"/>
+      <c r="F50" s="41"/>
     </row>
     <row r="51" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A51" s="10" t="s">
@@ -2088,8 +2088,8 @@
       <c r="D51" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="E51" s="31"/>
-      <c r="F51" s="31"/>
+      <c r="E51" s="41"/>
+      <c r="F51" s="41"/>
     </row>
     <row r="52" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A52" s="10" t="s">
@@ -2104,11 +2104,16 @@
       <c r="D52" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="E52" s="31"/>
-      <c r="F52" s="31"/>
+      <c r="E52" s="41"/>
+      <c r="F52" s="41"/>
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="E48:F48"/>
+    <mergeCell ref="E49:F49"/>
+    <mergeCell ref="E50:F50"/>
+    <mergeCell ref="E51:F51"/>
+    <mergeCell ref="E52:F52"/>
     <mergeCell ref="A40:D40"/>
     <mergeCell ref="B2:E2"/>
     <mergeCell ref="B4:E4"/>
@@ -2121,11 +2126,6 @@
     <mergeCell ref="B34:C37"/>
     <mergeCell ref="B38:C38"/>
     <mergeCell ref="B39:D39"/>
-    <mergeCell ref="E48:F48"/>
-    <mergeCell ref="E49:F49"/>
-    <mergeCell ref="E50:F50"/>
-    <mergeCell ref="E51:F51"/>
-    <mergeCell ref="E52:F52"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="63" orientation="portrait" r:id="rId1"/>

</xml_diff>